<commit_message>
Docs: Se crean las primeros 3 actores con sus tablas
</commit_message>
<xml_diff>
--- a/Creacion de users.xlsx
+++ b/Creacion de users.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lucho\Documents\GitHub\Repositorio-de-equipo-3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{282BCB59-88D4-42B2-889C-A44844A55C3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{346C4DFD-03C8-4064-B563-B9D35E993EB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="855" yWindow="-120" windowWidth="28065" windowHeight="16440" xr2:uid="{915D0D72-919F-4EC8-B87C-0E661B558825}"/>
+    <workbookView xWindow="14775" yWindow="0" windowWidth="14130" windowHeight="16305" xr2:uid="{915D0D72-919F-4EC8-B87C-0E661B558825}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,14 +34,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="36">
   <si>
     <t>Acceso total</t>
   </si>
   <si>
-    <t>PRIVILEGIOS</t>
-  </si>
-  <si>
     <t>TABLAS</t>
   </si>
   <si>
@@ -51,18 +48,12 @@
     <t>ACTORES</t>
   </si>
   <si>
-    <t>USUARIO</t>
-  </si>
-  <si>
     <t>CONTRASEÑA</t>
   </si>
   <si>
     <t>83LjlO9o/OIB1q)d</t>
   </si>
   <si>
-    <t>5.u[3iXxN!KIPWHp</t>
-  </si>
-  <si>
     <t>]e(@Wi/1GXL)GKzB</t>
   </si>
   <si>
@@ -81,18 +72,12 @@
     <t>EdwinCAbaunza</t>
   </si>
   <si>
-    <t>DavidSCruz</t>
-  </si>
-  <si>
     <t>LuisJMarino</t>
   </si>
   <si>
     <t>Create, Read, Update, Delete</t>
   </si>
   <si>
-    <t xml:space="preserve">Aprendiz </t>
-  </si>
-  <si>
     <t>Instructor</t>
   </si>
   <si>
@@ -102,29 +87,68 @@
     <t>Coordinador</t>
   </si>
   <si>
-    <t>vigilante de minutas</t>
-  </si>
-  <si>
     <t>aprendiz, ambientes, minutas, novedades, incidentes, asistencia, jornada</t>
   </si>
   <si>
-    <t>minuta de ambientes, equipos, ambientes, visitantes, incidentes, jornada</t>
-  </si>
-  <si>
     <t>Create, Read, Update</t>
   </si>
   <si>
-    <t>aprendiz, recursos, asistencia, modalidad, programas, coordinación, jornada</t>
-  </si>
-  <si>
     <t>maldito github</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> PRIVILEGIOS (PERMISOS) - CRUD</t>
+  </si>
+  <si>
+    <t>NOMBRE DE USUARIO</t>
+  </si>
+  <si>
+    <t>CODIGO MYSQL CREACIÓN USUARIO</t>
+  </si>
+  <si>
+    <t>CODIGO MYSQL ASIGNACION DE PERMISOS</t>
+  </si>
+  <si>
+    <t>Aprendiz</t>
+  </si>
+  <si>
+    <t>Asistencia</t>
+  </si>
+  <si>
+    <t>Incidente</t>
+  </si>
+  <si>
+    <t>Programas</t>
+  </si>
+  <si>
+    <t>Jornada</t>
+  </si>
+  <si>
+    <t>Modalidad</t>
+  </si>
+  <si>
+    <t>Read</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Read </t>
+  </si>
+  <si>
+    <t>Vigilante Minuta</t>
+  </si>
+  <si>
+    <t>Registro minuta</t>
+  </si>
+  <si>
+    <t>Ambiente</t>
+  </si>
+  <si>
+    <t>Recursos</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -139,8 +163,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -150,6 +181,30 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF008000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -180,9 +235,13 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top/>
-      <bottom/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -190,11 +249,43 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Bueno" xfId="1" builtinId="26"/>
@@ -202,6 +293,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF008000"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -510,127 +606,345 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{914852BE-CF9F-4359-89B7-1C4A7749B8FD}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:J35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.5703125" customWidth="1"/>
     <col min="2" max="2" width="17.42578125" customWidth="1"/>
-    <col min="3" max="3" width="21.85546875" customWidth="1"/>
-    <col min="4" max="4" width="102.85546875" customWidth="1"/>
-    <col min="5" max="5" width="31.5703125" customWidth="1"/>
+    <col min="3" max="3" width="31.28515625" customWidth="1"/>
+    <col min="4" max="4" width="77.5703125" customWidth="1"/>
+    <col min="5" max="5" width="22.5703125" customWidth="1"/>
+    <col min="6" max="6" width="36.42578125" customWidth="1"/>
+    <col min="7" max="7" width="20.5703125" customWidth="1"/>
+    <col min="8" max="8" width="8.28515625" customWidth="1"/>
+    <col min="10" max="10" width="13.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:10" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="F1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="6"/>
+      <c r="B3" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="6"/>
+      <c r="B4" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="6"/>
+      <c r="B5" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="6"/>
+      <c r="B6" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="6"/>
+      <c r="B7" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="8"/>
+      <c r="B9" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="8"/>
+      <c r="B10" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="8"/>
+      <c r="B11" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="15"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="15"/>
+      <c r="F12" s="15"/>
+      <c r="G12" s="15"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="14"/>
+      <c r="B13" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="14"/>
+      <c r="B14" s="15"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="15"/>
+      <c r="G14" s="15"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="14"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="14"/>
+      <c r="B16" s="15"/>
+      <c r="C16" s="15"/>
+      <c r="D16" s="15"/>
+      <c r="E16" s="15"/>
+      <c r="F16" s="15"/>
+      <c r="G16" s="15"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="14"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="14"/>
+      <c r="B18" s="15"/>
+      <c r="C18" s="15"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="15"/>
+      <c r="G18" s="15"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="14"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="12"/>
+      <c r="B30" s="12"/>
+      <c r="C30" s="12"/>
+      <c r="D30" s="12"/>
+      <c r="E30" s="12"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="13"/>
+      <c r="B31" s="13"/>
+      <c r="C31" s="13"/>
+      <c r="D31" s="13"/>
+      <c r="E31" s="13"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="13"/>
+      <c r="B32" s="13"/>
+      <c r="C32" s="13"/>
+      <c r="D32" s="13"/>
+      <c r="E32" s="13"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B33" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C33" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="D33" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E33" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="1" t="s">
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" s="1" t="s">
+      <c r="B35" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C35" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="D35" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="3"/>
+      <c r="E35" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A2:A7"/>
+    <mergeCell ref="A8:A11"/>
+    <mergeCell ref="A12:A19"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Docs: Actores, Tablas, Privilegios
</commit_message>
<xml_diff>
--- a/Creacion de users.xlsx
+++ b/Creacion de users.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lucho\Documents\GitHub\Repositorio-de-equipo-3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{346C4DFD-03C8-4064-B563-B9D35E993EB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1EE2019-D0B6-419C-8046-9D2FBA23A12C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14775" yWindow="0" windowWidth="14130" windowHeight="16305" xr2:uid="{915D0D72-919F-4EC8-B87C-0E661B558825}"/>
+    <workbookView xWindow="855" yWindow="-120" windowWidth="28065" windowHeight="16440" xr2:uid="{915D0D72-919F-4EC8-B87C-0E661B558825}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,10 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="36">
-  <si>
-    <t>Acceso total</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="29">
   <si>
     <t>TABLAS</t>
   </si>
@@ -51,30 +48,6 @@
     <t>CONTRASEÑA</t>
   </si>
   <si>
-    <t>83LjlO9o/OIB1q)d</t>
-  </si>
-  <si>
-    <t>]e(@Wi/1GXL)GKzB</t>
-  </si>
-  <si>
-    <t>dn(KLdDBhX47JLNx</t>
-  </si>
-  <si>
-    <t>hjUPSx_]zBuxh1p@</t>
-  </si>
-  <si>
-    <t>KennenSCortez</t>
-  </si>
-  <si>
-    <t>MahilyKGutierrez</t>
-  </si>
-  <si>
-    <t>EdwinCAbaunza</t>
-  </si>
-  <si>
-    <t>LuisJMarino</t>
-  </si>
-  <si>
     <t>Create, Read, Update, Delete</t>
   </si>
   <si>
@@ -87,15 +60,9 @@
     <t>Coordinador</t>
   </si>
   <si>
-    <t>aprendiz, ambientes, minutas, novedades, incidentes, asistencia, jornada</t>
-  </si>
-  <si>
     <t>Create, Read, Update</t>
   </si>
   <si>
-    <t>maldito github</t>
-  </si>
-  <si>
     <t xml:space="preserve"> PRIVILEGIOS (PERMISOS) - CRUD</t>
   </si>
   <si>
@@ -142,13 +109,25 @@
   </si>
   <si>
     <t>Recursos</t>
+  </si>
+  <si>
+    <t>Minutas</t>
+  </si>
+  <si>
+    <t>Novedades</t>
+  </si>
+  <si>
+    <t>Acceso Total</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -170,8 +149,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -207,8 +192,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC189F7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -238,6 +235,30 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top/>
       <bottom style="thin">
         <color indexed="64"/>
@@ -249,13 +270,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -279,13 +305,41 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Bueno" xfId="1" builtinId="26"/>
@@ -606,10 +660,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{914852BE-CF9F-4359-89B7-1C4A7749B8FD}">
-  <dimension ref="A1:J35"/>
+  <dimension ref="A1:P46"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="P13" sqref="P13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -625,325 +679,568 @@
     <col min="10" max="10" width="13.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:16" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="F1" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3" s="7"/>
+      <c r="B3" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4" s="7"/>
+      <c r="B4" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5" s="7"/>
+      <c r="B5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" s="7"/>
+      <c r="B6" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7" s="7"/>
+      <c r="B7" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="B8" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9" s="9"/>
+      <c r="B9" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10" s="9"/>
+      <c r="B10" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11"/>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11" s="9"/>
+      <c r="B11" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A12" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" s="17"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="17"/>
+      <c r="G12" s="17"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A13" s="15"/>
+      <c r="B13" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="P13" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14" s="15"/>
+      <c r="B14" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" s="17"/>
+      <c r="E14" s="17"/>
+      <c r="F14" s="17"/>
+      <c r="G14" s="17"/>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A15" s="15"/>
+      <c r="B15" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A16" s="15"/>
+      <c r="B16" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16" s="17"/>
+      <c r="E16" s="17"/>
+      <c r="F16" s="17"/>
+      <c r="G16" s="17"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="15"/>
+      <c r="B17" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="15"/>
+      <c r="B18" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="C18" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="D18" s="17"/>
+      <c r="E18" s="17"/>
+      <c r="F18" s="17"/>
+      <c r="G18" s="17"/>
+      <c r="H18" s="12"/>
+      <c r="I18" s="12"/>
+      <c r="J18" s="12"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="16"/>
+      <c r="B19" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="C19" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="D19" s="21"/>
+      <c r="E19" s="21"/>
+      <c r="F19" s="21"/>
+      <c r="G19" s="21"/>
+      <c r="H19" s="12"/>
+      <c r="I19" s="12"/>
+      <c r="J19" s="12"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="G1" s="5" t="s">
+      <c r="D20" s="19"/>
+      <c r="E20" s="19"/>
+      <c r="F20" s="19"/>
+      <c r="G20" s="19"/>
+      <c r="H20" s="12"/>
+      <c r="I20" s="12"/>
+      <c r="J20" s="12"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="19"/>
+      <c r="B21" s="19"/>
+      <c r="C21" s="19"/>
+      <c r="D21" s="19"/>
+      <c r="E21" s="19"/>
+      <c r="F21" s="19"/>
+      <c r="G21" s="19"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="19"/>
+      <c r="B22" s="19"/>
+      <c r="C22" s="19"/>
+      <c r="D22" s="19"/>
+      <c r="E22" s="19"/>
+      <c r="F22" s="19"/>
+      <c r="G22" s="19"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" s="23"/>
+      <c r="B24" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="C24" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="D24" s="24"/>
+      <c r="E24" s="24"/>
+      <c r="F24" s="24"/>
+      <c r="G24" s="24"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" s="23"/>
+      <c r="B25" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" s="23"/>
+      <c r="B26" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="C26" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="D26" s="24"/>
+      <c r="E26" s="24"/>
+      <c r="F26" s="24"/>
+      <c r="G26" s="24"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" s="23"/>
+      <c r="B27" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" s="23"/>
+      <c r="B28" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="C28" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="D28" s="24"/>
+      <c r="E28" s="24"/>
+      <c r="F28" s="24"/>
+      <c r="G28" s="24"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" s="23"/>
+      <c r="B29" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="6"/>
-      <c r="B3" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="6"/>
-      <c r="B4" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="6"/>
-      <c r="B5" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="6"/>
-      <c r="B6" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="6"/>
-      <c r="B7" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="B8" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="C8" s="10" t="s">
+      <c r="C29" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
+      <c r="G29" s="3"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" s="23"/>
+      <c r="B30" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="C30" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="D30" s="24"/>
+      <c r="E30" s="24"/>
+      <c r="F30" s="24"/>
+      <c r="G30" s="24"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" s="23"/>
+      <c r="B31" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="8"/>
-      <c r="B9" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="8"/>
-      <c r="B10" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="C10" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="10"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="8"/>
-      <c r="B11" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="C12" s="15"/>
-      <c r="D12" s="15"/>
-      <c r="E12" s="15"/>
-      <c r="F12" s="15"/>
-      <c r="G12" s="15"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="14"/>
-      <c r="B13" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="14"/>
-      <c r="B14" s="15"/>
-      <c r="C14" s="15"/>
-      <c r="D14" s="15"/>
-      <c r="E14" s="15"/>
-      <c r="F14" s="15"/>
-      <c r="G14" s="15"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="14"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="14"/>
-      <c r="B16" s="15"/>
-      <c r="C16" s="15"/>
-      <c r="D16" s="15"/>
-      <c r="E16" s="15"/>
-      <c r="F16" s="15"/>
-      <c r="G16" s="15"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="14"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="14"/>
-      <c r="B18" s="15"/>
-      <c r="C18" s="15"/>
-      <c r="D18" s="15"/>
-      <c r="E18" s="15"/>
-      <c r="F18" s="15"/>
-      <c r="G18" s="15"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="14"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="12"/>
-      <c r="B30" s="12"/>
-      <c r="C30" s="12"/>
-      <c r="D30" s="12"/>
-      <c r="E30" s="12"/>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="13"/>
-      <c r="B31" s="13"/>
-      <c r="C31" s="13"/>
-      <c r="D31" s="13"/>
-      <c r="E31" s="13"/>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C31" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D31" s="20"/>
+      <c r="E31" s="20"/>
+      <c r="F31" s="3"/>
+      <c r="G31" s="3"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="13"/>
       <c r="B32" s="13"/>
       <c r="C32" s="13"/>
       <c r="D32" s="13"/>
       <c r="E32" s="13"/>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="B33" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C33" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="D33" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="E33" s="11" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E35" s="1" t="s">
-        <v>18</v>
-      </c>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="13"/>
+      <c r="B33" s="13"/>
+      <c r="C33" s="13"/>
+      <c r="D33" s="13"/>
+      <c r="E33" s="13"/>
+      <c r="F33" s="13"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="13"/>
+      <c r="B34" s="13"/>
+      <c r="C34" s="13"/>
+      <c r="D34" s="13"/>
+      <c r="E34" s="13"/>
+      <c r="F34" s="13"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="13"/>
+      <c r="B35" s="13"/>
+      <c r="C35" s="13"/>
+      <c r="D35" s="13"/>
+      <c r="E35" s="13"/>
+      <c r="F35" s="13"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="13"/>
+      <c r="B36" s="13"/>
+      <c r="C36" s="13"/>
+      <c r="D36" s="13"/>
+      <c r="E36" s="13"/>
+      <c r="F36" s="13"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="13"/>
+      <c r="B37" s="13"/>
+      <c r="C37" s="13"/>
+      <c r="D37" s="13"/>
+      <c r="E37" s="13"/>
+      <c r="F37" s="13"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="13"/>
+      <c r="B38" s="13"/>
+      <c r="C38" s="13"/>
+      <c r="D38" s="13"/>
+      <c r="E38" s="13"/>
+      <c r="F38" s="13"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="13"/>
+      <c r="B39" s="13"/>
+      <c r="C39" s="13"/>
+      <c r="D39" s="13"/>
+      <c r="E39" s="13"/>
+      <c r="F39" s="13"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="13"/>
+      <c r="B40" s="13"/>
+      <c r="C40" s="13"/>
+      <c r="D40" s="13"/>
+      <c r="E40" s="13"/>
+      <c r="F40" s="13"/>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="13"/>
+      <c r="B41" s="13"/>
+      <c r="C41" s="13"/>
+      <c r="D41" s="13"/>
+      <c r="E41" s="13"/>
+      <c r="F41" s="13"/>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" s="13"/>
+      <c r="B42" s="13"/>
+      <c r="C42" s="13"/>
+      <c r="D42" s="13"/>
+      <c r="E42" s="13"/>
+      <c r="F42" s="13"/>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" s="13"/>
+      <c r="B43" s="13"/>
+      <c r="C43" s="13"/>
+      <c r="D43" s="13"/>
+      <c r="E43" s="13"/>
+      <c r="F43" s="13"/>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" s="13"/>
+      <c r="B44" s="13"/>
+      <c r="C44" s="13"/>
+      <c r="D44" s="13"/>
+      <c r="E44" s="13"/>
+      <c r="F44" s="13"/>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" s="13"/>
+      <c r="B45" s="13"/>
+      <c r="C45" s="13"/>
+      <c r="D45" s="13"/>
+      <c r="E45" s="13"/>
+      <c r="F45" s="13"/>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" s="13"/>
+      <c r="B46" s="13"/>
+      <c r="C46" s="13"/>
+      <c r="D46" s="13"/>
+      <c r="E46" s="13"/>
+      <c r="F46" s="13"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="11">
+    <mergeCell ref="D20:D22"/>
+    <mergeCell ref="E20:E22"/>
+    <mergeCell ref="F20:F22"/>
+    <mergeCell ref="G20:G22"/>
+    <mergeCell ref="A23:A31"/>
     <mergeCell ref="A2:A7"/>
     <mergeCell ref="A8:A11"/>
     <mergeCell ref="A12:A19"/>
+    <mergeCell ref="A20:A22"/>
+    <mergeCell ref="B20:B22"/>
+    <mergeCell ref="C20:C22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Docs: Actores, Tablas, Privilegios, Nombre de usuario
</commit_message>
<xml_diff>
--- a/Creacion de users.xlsx
+++ b/Creacion de users.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lucho\Documents\GitHub\Repositorio-de-equipo-3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1EE2019-D0B6-419C-8046-9D2FBA23A12C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB7972BE-86F2-4409-812F-C7DB4110F68C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="855" yWindow="-120" windowWidth="28065" windowHeight="16440" xr2:uid="{915D0D72-919F-4EC8-B87C-0E661B558825}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="34">
   <si>
     <t>TABLAS</t>
   </si>
@@ -48,6 +48,18 @@
     <t>CONTRASEÑA</t>
   </si>
   <si>
+    <t>MahilyKGutierrez</t>
+  </si>
+  <si>
+    <t>EdwinCAbaunza</t>
+  </si>
+  <si>
+    <t>DavidSCruz</t>
+  </si>
+  <si>
+    <t>LuisJMarino</t>
+  </si>
+  <si>
     <t>Create, Read, Update, Delete</t>
   </si>
   <si>
@@ -121,6 +133,9 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>KennenSCortés</t>
   </si>
 </sst>
 </file>
@@ -270,16 +285,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -325,20 +337,20 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -662,8 +674,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{914852BE-CF9F-4359-89B7-1C4A7749B8FD}">
   <dimension ref="A1:P46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="P13" sqref="P13"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -671,7 +683,7 @@
     <col min="1" max="1" width="23.5703125" customWidth="1"/>
     <col min="2" max="2" width="17.42578125" customWidth="1"/>
     <col min="3" max="3" width="31.28515625" customWidth="1"/>
-    <col min="4" max="4" width="77.5703125" customWidth="1"/>
+    <col min="4" max="4" width="29" customWidth="1"/>
     <col min="5" max="5" width="22.5703125" customWidth="1"/>
     <col min="6" max="6" width="36.42578125" customWidth="1"/>
     <col min="7" max="7" width="20.5703125" customWidth="1"/>
@@ -680,216 +692,222 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E1" s="6" t="s">
+      <c r="C1" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>12</v>
+      <c r="F1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>16</v>
       </c>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" s="8" t="s">
+      <c r="A2" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
+      <c r="D2" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="9"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" s="7"/>
-      <c r="B3" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" s="4" t="s">
+      <c r="A3" s="6"/>
+      <c r="B3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4" s="6"/>
+      <c r="B4" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5" s="6"/>
+      <c r="B5" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4" s="7"/>
-      <c r="B4" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="8" t="s">
+      <c r="C5" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" s="6"/>
+      <c r="B6" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7" s="6"/>
+      <c r="B7" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10"/>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9" s="8"/>
+      <c r="B9" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" s="7"/>
-      <c r="B5" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" s="7"/>
-      <c r="B6" s="8" t="s">
+      <c r="C9" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10" s="8"/>
+      <c r="B10" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11" s="8"/>
+      <c r="B11" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A12" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" s="7"/>
-      <c r="B7" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A8" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="C8" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="11"/>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9" s="9"/>
-      <c r="B9" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A10" s="9"/>
-      <c r="B10" s="11" t="s">
+      <c r="C12" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="11"/>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A11" s="9"/>
-      <c r="B11" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A12" s="14" t="s">
+      <c r="D12" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="B12" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="C12" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="D12" s="17"/>
-      <c r="E12" s="17"/>
-      <c r="F12" s="17"/>
-      <c r="G12" s="17"/>
+      <c r="E12" s="16"/>
+      <c r="F12" s="16"/>
+      <c r="G12" s="16"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A13" s="15"/>
+      <c r="A13" s="14"/>
       <c r="B13" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>23</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>19</v>
       </c>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
       <c r="P13" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A14" s="15"/>
-      <c r="B14" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="C14" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="D14" s="17"/>
-      <c r="E14" s="17"/>
-      <c r="F14" s="17"/>
-      <c r="G14" s="17"/>
+      <c r="A14" s="14"/>
+      <c r="B14" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" s="16"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="16"/>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A15" s="15"/>
+      <c r="A15" s="14"/>
       <c r="B15" s="2" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
@@ -897,134 +915,138 @@
       <c r="G15" s="2"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A16" s="15"/>
-      <c r="B16" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="C16" s="17" t="s">
+      <c r="A16" s="14"/>
+      <c r="B16" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="D16" s="16"/>
+      <c r="E16" s="16"/>
+      <c r="F16" s="16"/>
+      <c r="G16" s="16"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="14"/>
+      <c r="B17" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="D17" s="17"/>
+      <c r="E17" s="17"/>
+      <c r="F17" s="17"/>
+      <c r="G17" s="17"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="14"/>
+      <c r="B18" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="D18" s="16"/>
+      <c r="E18" s="16"/>
+      <c r="F18" s="16"/>
+      <c r="G18" s="16"/>
+      <c r="H18" s="11"/>
+      <c r="I18" s="11"/>
+      <c r="J18" s="11"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="15"/>
+      <c r="B19" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="C19" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="D19" s="19"/>
+      <c r="E19" s="19"/>
+      <c r="F19" s="19"/>
+      <c r="G19" s="19"/>
+      <c r="H19" s="11"/>
+      <c r="I19" s="11"/>
+      <c r="J19" s="11"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="B20" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="C20" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="D16" s="17"/>
-      <c r="E16" s="17"/>
-      <c r="F16" s="17"/>
-      <c r="G16" s="17"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="15"/>
-      <c r="B17" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="C17" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="D17" s="18"/>
-      <c r="E17" s="18"/>
-      <c r="F17" s="18"/>
-      <c r="G17" s="18"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="15"/>
-      <c r="B18" s="17" t="s">
+      <c r="D20" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="E20" s="18"/>
+      <c r="F20" s="18"/>
+      <c r="G20" s="18"/>
+      <c r="H20" s="11"/>
+      <c r="I20" s="11"/>
+      <c r="J20" s="11"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="18"/>
+      <c r="B21" s="18"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="18"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="18"/>
+      <c r="B22" s="18"/>
+      <c r="C22" s="18"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="18"/>
+      <c r="G22" s="18"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="B23" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C18" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="D18" s="17"/>
-      <c r="E18" s="17"/>
-      <c r="F18" s="17"/>
-      <c r="G18" s="17"/>
-      <c r="H18" s="12"/>
-      <c r="I18" s="12"/>
-      <c r="J18" s="12"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="16"/>
-      <c r="B19" s="21" t="s">
-        <v>24</v>
-      </c>
-      <c r="C19" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="D19" s="21"/>
-      <c r="E19" s="21"/>
-      <c r="F19" s="21"/>
-      <c r="G19" s="21"/>
-      <c r="H19" s="12"/>
-      <c r="I19" s="12"/>
-      <c r="J19" s="12"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="B20" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="C20" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="D20" s="19"/>
-      <c r="E20" s="19"/>
-      <c r="F20" s="19"/>
-      <c r="G20" s="19"/>
-      <c r="H20" s="12"/>
-      <c r="I20" s="12"/>
-      <c r="J20" s="12"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="19"/>
-      <c r="B21" s="19"/>
-      <c r="C21" s="19"/>
-      <c r="D21" s="19"/>
-      <c r="E21" s="19"/>
-      <c r="F21" s="19"/>
-      <c r="G21" s="19"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="19"/>
-      <c r="B22" s="19"/>
-      <c r="C22" s="19"/>
-      <c r="D22" s="19"/>
-      <c r="E22" s="19"/>
-      <c r="F22" s="19"/>
-      <c r="G22" s="19"/>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="23" t="s">
-        <v>7</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>13</v>
-      </c>
       <c r="C23" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D23" s="3"/>
+        <v>12</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>33</v>
+      </c>
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="23"/>
-      <c r="B24" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="C24" s="24" t="s">
-        <v>8</v>
-      </c>
-      <c r="D24" s="24"/>
-      <c r="E24" s="24"/>
-      <c r="F24" s="24"/>
-      <c r="G24" s="24"/>
+      <c r="A24" s="20"/>
+      <c r="B24" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="C24" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="D24" s="21"/>
+      <c r="E24" s="21"/>
+      <c r="F24" s="21"/>
+      <c r="G24" s="21"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="23"/>
+      <c r="A25" s="20"/>
       <c r="B25" s="3" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
@@ -1032,25 +1054,25 @@
       <c r="G25" s="3"/>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="23"/>
-      <c r="B26" s="24" t="s">
-        <v>15</v>
-      </c>
-      <c r="C26" s="24" t="s">
-        <v>8</v>
-      </c>
-      <c r="D26" s="24"/>
-      <c r="E26" s="24"/>
-      <c r="F26" s="24"/>
-      <c r="G26" s="24"/>
+      <c r="A26" s="20"/>
+      <c r="B26" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="C26" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="D26" s="21"/>
+      <c r="E26" s="21"/>
+      <c r="F26" s="21"/>
+      <c r="G26" s="21"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="23"/>
+      <c r="A27" s="20"/>
       <c r="B27" s="3" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D27" s="3"/>
       <c r="E27" s="3"/>
@@ -1058,25 +1080,25 @@
       <c r="G27" s="3"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" s="23"/>
-      <c r="B28" s="24" t="s">
-        <v>23</v>
-      </c>
-      <c r="C28" s="24" t="s">
-        <v>8</v>
-      </c>
-      <c r="D28" s="24"/>
-      <c r="E28" s="24"/>
-      <c r="F28" s="24"/>
-      <c r="G28" s="24"/>
+      <c r="A28" s="20"/>
+      <c r="B28" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="C28" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="D28" s="21"/>
+      <c r="E28" s="21"/>
+      <c r="F28" s="21"/>
+      <c r="G28" s="21"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" s="23"/>
+      <c r="A29" s="20"/>
       <c r="B29" s="3" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D29" s="3"/>
       <c r="E29" s="3"/>
@@ -1084,149 +1106,149 @@
       <c r="G29" s="3"/>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" s="23"/>
-      <c r="B30" s="24" t="s">
-        <v>17</v>
-      </c>
-      <c r="C30" s="24" t="s">
-        <v>8</v>
-      </c>
-      <c r="D30" s="24"/>
-      <c r="E30" s="24"/>
-      <c r="F30" s="24"/>
-      <c r="G30" s="24"/>
+      <c r="A30" s="20"/>
+      <c r="B30" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="C30" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="D30" s="21"/>
+      <c r="E30" s="21"/>
+      <c r="F30" s="21"/>
+      <c r="G30" s="21"/>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" s="23"/>
+      <c r="A31" s="20"/>
       <c r="B31" s="22" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D31" s="20"/>
-      <c r="E31" s="20"/>
+        <v>12</v>
+      </c>
+      <c r="D31" s="23"/>
+      <c r="E31" s="23"/>
       <c r="F31" s="3"/>
       <c r="G31" s="3"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32" s="13"/>
-      <c r="B32" s="13"/>
-      <c r="C32" s="13"/>
-      <c r="D32" s="13"/>
-      <c r="E32" s="13"/>
+      <c r="A32" s="12"/>
+      <c r="B32" s="12"/>
+      <c r="C32" s="12"/>
+      <c r="D32" s="12"/>
+      <c r="E32" s="12"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="13"/>
-      <c r="B33" s="13"/>
-      <c r="C33" s="13"/>
-      <c r="D33" s="13"/>
-      <c r="E33" s="13"/>
-      <c r="F33" s="13"/>
+      <c r="A33" s="12"/>
+      <c r="B33" s="12"/>
+      <c r="C33" s="12"/>
+      <c r="D33" s="12"/>
+      <c r="E33" s="12"/>
+      <c r="F33" s="12"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="13"/>
-      <c r="B34" s="13"/>
-      <c r="C34" s="13"/>
-      <c r="D34" s="13"/>
-      <c r="E34" s="13"/>
-      <c r="F34" s="13"/>
+      <c r="A34" s="12"/>
+      <c r="B34" s="12"/>
+      <c r="C34" s="12"/>
+      <c r="D34" s="12"/>
+      <c r="E34" s="12"/>
+      <c r="F34" s="12"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="13"/>
-      <c r="B35" s="13"/>
-      <c r="C35" s="13"/>
-      <c r="D35" s="13"/>
-      <c r="E35" s="13"/>
-      <c r="F35" s="13"/>
+      <c r="A35" s="12"/>
+      <c r="B35" s="12"/>
+      <c r="C35" s="12"/>
+      <c r="D35" s="12"/>
+      <c r="E35" s="12"/>
+      <c r="F35" s="12"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="13"/>
-      <c r="B36" s="13"/>
-      <c r="C36" s="13"/>
-      <c r="D36" s="13"/>
-      <c r="E36" s="13"/>
-      <c r="F36" s="13"/>
+      <c r="A36" s="12"/>
+      <c r="B36" s="12"/>
+      <c r="C36" s="12"/>
+      <c r="D36" s="12"/>
+      <c r="E36" s="12"/>
+      <c r="F36" s="12"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="13"/>
-      <c r="B37" s="13"/>
-      <c r="C37" s="13"/>
-      <c r="D37" s="13"/>
-      <c r="E37" s="13"/>
-      <c r="F37" s="13"/>
+      <c r="A37" s="12"/>
+      <c r="B37" s="12"/>
+      <c r="C37" s="12"/>
+      <c r="D37" s="12"/>
+      <c r="E37" s="12"/>
+      <c r="F37" s="12"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="13"/>
-      <c r="B38" s="13"/>
-      <c r="C38" s="13"/>
-      <c r="D38" s="13"/>
-      <c r="E38" s="13"/>
-      <c r="F38" s="13"/>
+      <c r="A38" s="12"/>
+      <c r="B38" s="12"/>
+      <c r="C38" s="12"/>
+      <c r="D38" s="12"/>
+      <c r="E38" s="12"/>
+      <c r="F38" s="12"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="13"/>
-      <c r="B39" s="13"/>
-      <c r="C39" s="13"/>
-      <c r="D39" s="13"/>
-      <c r="E39" s="13"/>
-      <c r="F39" s="13"/>
+      <c r="A39" s="12"/>
+      <c r="B39" s="12"/>
+      <c r="C39" s="12"/>
+      <c r="D39" s="12"/>
+      <c r="E39" s="12"/>
+      <c r="F39" s="12"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="13"/>
-      <c r="B40" s="13"/>
-      <c r="C40" s="13"/>
-      <c r="D40" s="13"/>
-      <c r="E40" s="13"/>
-      <c r="F40" s="13"/>
+      <c r="A40" s="12"/>
+      <c r="B40" s="12"/>
+      <c r="C40" s="12"/>
+      <c r="D40" s="12"/>
+      <c r="E40" s="12"/>
+      <c r="F40" s="12"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="13"/>
-      <c r="B41" s="13"/>
-      <c r="C41" s="13"/>
-      <c r="D41" s="13"/>
-      <c r="E41" s="13"/>
-      <c r="F41" s="13"/>
+      <c r="A41" s="12"/>
+      <c r="B41" s="12"/>
+      <c r="C41" s="12"/>
+      <c r="D41" s="12"/>
+      <c r="E41" s="12"/>
+      <c r="F41" s="12"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="13"/>
-      <c r="B42" s="13"/>
-      <c r="C42" s="13"/>
-      <c r="D42" s="13"/>
-      <c r="E42" s="13"/>
-      <c r="F42" s="13"/>
+      <c r="A42" s="12"/>
+      <c r="B42" s="12"/>
+      <c r="C42" s="12"/>
+      <c r="D42" s="12"/>
+      <c r="E42" s="12"/>
+      <c r="F42" s="12"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="13"/>
-      <c r="B43" s="13"/>
-      <c r="C43" s="13"/>
-      <c r="D43" s="13"/>
-      <c r="E43" s="13"/>
-      <c r="F43" s="13"/>
+      <c r="A43" s="12"/>
+      <c r="B43" s="12"/>
+      <c r="C43" s="12"/>
+      <c r="D43" s="12"/>
+      <c r="E43" s="12"/>
+      <c r="F43" s="12"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="13"/>
-      <c r="B44" s="13"/>
-      <c r="C44" s="13"/>
-      <c r="D44" s="13"/>
-      <c r="E44" s="13"/>
-      <c r="F44" s="13"/>
+      <c r="A44" s="12"/>
+      <c r="B44" s="12"/>
+      <c r="C44" s="12"/>
+      <c r="D44" s="12"/>
+      <c r="E44" s="12"/>
+      <c r="F44" s="12"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="13"/>
-      <c r="B45" s="13"/>
-      <c r="C45" s="13"/>
-      <c r="D45" s="13"/>
-      <c r="E45" s="13"/>
-      <c r="F45" s="13"/>
+      <c r="A45" s="12"/>
+      <c r="B45" s="12"/>
+      <c r="C45" s="12"/>
+      <c r="D45" s="12"/>
+      <c r="E45" s="12"/>
+      <c r="F45" s="12"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="13"/>
-      <c r="B46" s="13"/>
-      <c r="C46" s="13"/>
-      <c r="D46" s="13"/>
-      <c r="E46" s="13"/>
-      <c r="F46" s="13"/>
+      <c r="A46" s="12"/>
+      <c r="B46" s="12"/>
+      <c r="C46" s="12"/>
+      <c r="D46" s="12"/>
+      <c r="E46" s="12"/>
+      <c r="F46" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="11">

</xml_diff>

<commit_message>
Docs: Creacion completa de la tabla
 en el codigo mySQL de permisos en la parte de administrador, esta vacio, tengo que preguntar a la profesora
</commit_message>
<xml_diff>
--- a/Creacion de users.xlsx
+++ b/Creacion de users.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lucho\Documents\GitHub\Repositorio-de-equipo-3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB7972BE-86F2-4409-812F-C7DB4110F68C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{293A9A32-9697-4595-8E3B-962225E2FC22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="855" yWindow="-120" windowWidth="28065" windowHeight="16440" xr2:uid="{915D0D72-919F-4EC8-B87C-0E661B558825}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="69">
   <si>
     <t>TABLAS</t>
   </si>
@@ -126,9 +126,6 @@
     <t>Minutas</t>
   </si>
   <si>
-    <t>Novedades</t>
-  </si>
-  <si>
     <t>Acceso Total</t>
   </si>
   <si>
@@ -136,13 +133,121 @@
   </si>
   <si>
     <t>KennenSCortés</t>
+  </si>
+  <si>
+    <t>M@hilyK2025!</t>
+  </si>
+  <si>
+    <t>D4v1dSC#08</t>
+  </si>
+  <si>
+    <t>E.CamiloA$92</t>
+  </si>
+  <si>
+    <t>Vol1Bear_LJM</t>
+  </si>
+  <si>
+    <t>KennenStorm#SC</t>
+  </si>
+  <si>
+    <t>CREATE USER 'MahilyKGutierrez'@'localhost' IDENTIFIED BY 'M@hilyK2025!';</t>
+  </si>
+  <si>
+    <t>CREATE USER 'DavidSCruz'@'localhost' IDENTIFIED BY 'D4v1dSC#08';</t>
+  </si>
+  <si>
+    <t>CREATE USER 'EdwinCAbaunza'@'localhost' IDENTIFIED BY 'E.CamiloA$92';</t>
+  </si>
+  <si>
+    <t>CREATE USER 'santiago.cruzuwu25'@'localhost' IDENTIFIED BY 'Vol1Bear_LJM';</t>
+  </si>
+  <si>
+    <t>CREATE USER 'KennenSCortés'@'localhost' IDENTIFIED BY 'KennenStorm#SC';</t>
+  </si>
+  <si>
+    <t>GRANT SELECT, UPDATE ON sena.aprendiz TO 'MahilyKGutierrez'@'localhost'; FLUSH PRIVILEGES;</t>
+  </si>
+  <si>
+    <t>GRANT SELECT, UPDATE ON sena.asistencia TO 'MahilyKGutierrez'@'localhost'; FLUSH PRIVILEGES;</t>
+  </si>
+  <si>
+    <t>GRANT SELECT, UPDATE ON sena.incidente TO 'MahilyKGutierrez'@'localhost'; FLUSH PRIVILEGES;</t>
+  </si>
+  <si>
+    <t>GRANT SELECT, UPDATE ON sena.programas TO 'MahilyKGutierrez'@'localhost'; FLUSH PRIVILEGES;</t>
+  </si>
+  <si>
+    <t>GRANT SELECT, UPDATE ON sena.jornada TO 'MahilyKGutierrez'@'localhost'; FLUSH PRIVILEGES;</t>
+  </si>
+  <si>
+    <t>GRANT SELECT, UPDATE ON sena.modalidad TO 'MahilyKGutierrez'@'localhost'; FLUSH PRIVILEGES;</t>
+  </si>
+  <si>
+    <t>GRANT SELECT, UPDATE ON sena.registro_minuta TO 'DavidSCruz'@'localhost'; FLUSH PRIVILEGES;</t>
+  </si>
+  <si>
+    <t>GRANT SELECT, UPDATE ON sena.incidente TO 'DavidSCruz'@'localhost'; FLUSH PRIVILEGES;</t>
+  </si>
+  <si>
+    <t>GRANT SELECT, UPDATE ON sena.ambiente TO 'DavidSCruz'@'localhost'; FLUSH PRIVILEGES;</t>
+  </si>
+  <si>
+    <t>GRANT SELECT, UPDATE ON sena.recursos TO 'DavidSCruz'@'localhost'; FLUSH PRIVILEGES;</t>
+  </si>
+  <si>
+    <t>GRANT SELECT, UPDATE ON sena.recursos TO 'EdwinCAbaunza'@'localhost'; FLUSH PRIVILEGES;</t>
+  </si>
+  <si>
+    <t>GRANT SELECT, UPDATE ON sena.aprendiz TO 'EdwinCAbaunza'@'localhost'; FLUSH PRIVILEGES;</t>
+  </si>
+  <si>
+    <t>GRANT SELECT, UPDATE ON sena.ambiente TO 'EdwinCAbaunza'@'localhost'; FLUSH PRIVILEGES;</t>
+  </si>
+  <si>
+    <t>GRANT SELECT, UPDATE ON sena.minutas TO 'EdwinCAbaunza'@'localhost'; FLUSH PRIVILEGES;</t>
+  </si>
+  <si>
+    <t>GRANT SELECT, UPDATE ON sena.incidente TO 'EdwinCAbaunza'@'localhost'; FLUSH PRIVILEGES;</t>
+  </si>
+  <si>
+    <t>GRANT SELECT, UPDATE ON sena.asistencia TO 'EdwinCAbaunza'@'localhost'; FLUSH PRIVILEGES;</t>
+  </si>
+  <si>
+    <t>GRANT SELECT, UPDATE ON sena.jornada TO 'EdwinCAbaunza'@'localhost'; FLUSH PRIVILEGES;</t>
+  </si>
+  <si>
+    <t>GRANT SELECT, UPDATE ON sena.aprendiz TO 'KennenSCortés'@'localhost'; FLUSH PRIVILEGES;</t>
+  </si>
+  <si>
+    <t>GRANT SELECT, UPDATE ON sena.asistencia TO 'KennenSCortés'@'localhost'; FLUSH PRIVILEGES;</t>
+  </si>
+  <si>
+    <t>GRANT SELECT, UPDATE ON sena.programas TO 'KennenSCortés'@'localhost'; FLUSH PRIVILEGES;</t>
+  </si>
+  <si>
+    <t>GRANT SELECT, UPDATE ON sena.incidente TO 'KennenSCortés'@'localhost'; FLUSH PRIVILEGES;</t>
+  </si>
+  <si>
+    <t>GRANT SELECT, UPDATE ON sena.minutas TO 'KennenSCortés'@'localhost'; FLUSH PRIVILEGES;</t>
+  </si>
+  <si>
+    <t>GRANT SELECT, UPDATE ON sena.ambiente TO 'KennenSCortés'@'localhost'; FLUSH PRIVILEGES;</t>
+  </si>
+  <si>
+    <t>GRANT SELECT, UPDATE ON sena.recursos TO 'KennenSCortés'@'localhost'; FLUSH PRIVILEGES;</t>
+  </si>
+  <si>
+    <t>GRANT SELECT, UPDATE ON sena.jornada TO 'KennenSCortés'@'localhost'; FLUSH PRIVILEGES;</t>
+  </si>
+  <si>
+    <t>GRANT SELECT, UPDATE ON sena.modalidad TO 'KennenSCortés'@'localhost'; FLUSH PRIVILEGES;</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -170,8 +275,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -216,6 +329,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC189F7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -281,21 +400,28 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -310,9 +436,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -328,17 +451,11 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -352,9 +469,28 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Bueno" xfId="1" builtinId="26"/>
+    <cellStyle name="Hipervínculo" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -672,10 +808,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{914852BE-CF9F-4359-89B7-1C4A7749B8FD}">
-  <dimension ref="A1:P46"/>
+  <dimension ref="A1:P45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="N25" sqref="N25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -686,584 +822,646 @@
     <col min="4" max="4" width="29" customWidth="1"/>
     <col min="5" max="5" width="22.5703125" customWidth="1"/>
     <col min="6" max="6" width="36.42578125" customWidth="1"/>
-    <col min="7" max="7" width="20.5703125" customWidth="1"/>
+    <col min="7" max="7" width="39" customWidth="1"/>
     <col min="8" max="8" width="8.28515625" customWidth="1"/>
     <col min="10" max="10" width="13.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+    </row>
+    <row r="2" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D2" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="9"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" s="6"/>
-      <c r="B3" s="3" t="s">
+      <c r="E2" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="F2" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="G2" s="24" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" ht="60" x14ac:dyDescent="0.25">
+      <c r="A3" s="8"/>
+      <c r="B3" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4" s="6"/>
-      <c r="B4" s="7" t="s">
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" ht="60" x14ac:dyDescent="0.25">
+      <c r="A4" s="8"/>
+      <c r="B4" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" s="6"/>
-      <c r="B5" s="3" t="s">
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="24" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" ht="60" x14ac:dyDescent="0.25">
+      <c r="A5" s="8"/>
+      <c r="B5" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" s="6"/>
-      <c r="B6" s="7" t="s">
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="8"/>
+      <c r="B6" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" s="6"/>
-      <c r="B7" s="3" t="s">
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="24" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" ht="60" x14ac:dyDescent="0.25">
+      <c r="A7" s="8"/>
+      <c r="B7" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" ht="60" x14ac:dyDescent="0.25">
+      <c r="A8" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="D8" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9" s="8"/>
-      <c r="B9" s="3" t="s">
+      <c r="E8" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="F8" s="25" t="s">
+        <v>39</v>
+      </c>
+      <c r="G8" s="25" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" ht="60" x14ac:dyDescent="0.25">
+      <c r="A9" s="10"/>
+      <c r="B9" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
       <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A10" s="8"/>
-      <c r="B10" s="10" t="s">
+      <c r="G9" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" ht="60" x14ac:dyDescent="0.25">
+      <c r="A10" s="10"/>
+      <c r="B10" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="C10" s="10" t="s">
+      <c r="C10" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="10"/>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A11" s="8"/>
-      <c r="B11" s="3" t="s">
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="25" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="10"/>
+      <c r="B11" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A12" s="13" t="s">
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="16" t="s">
+      <c r="B12" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="16" t="s">
+      <c r="C12" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="D12" s="16" t="s">
+      <c r="D12" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="E12" s="16"/>
-      <c r="F12" s="16"/>
-      <c r="G12" s="16"/>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A13" s="14"/>
-      <c r="B13" s="2" t="s">
+      <c r="E12" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="F12" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="G12" s="23" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" ht="60" x14ac:dyDescent="0.25">
+      <c r="A13" s="15"/>
+      <c r="B13" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="5" t="s">
+        <v>55</v>
+      </c>
       <c r="P13" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+      <c r="A14" s="15"/>
+      <c r="B14" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" s="23"/>
+      <c r="E14" s="23"/>
+      <c r="F14" s="23"/>
+      <c r="G14" s="23" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" ht="60" x14ac:dyDescent="0.25">
+      <c r="A15" s="15"/>
+      <c r="B15" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" ht="60" x14ac:dyDescent="0.25">
+      <c r="A16" s="15"/>
+      <c r="B16" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="23" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A17" s="15"/>
+      <c r="B17" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="H17" s="12"/>
+      <c r="I17" s="12"/>
+      <c r="J17" s="12"/>
+    </row>
+    <row r="18" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A18" s="16"/>
+      <c r="B18" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="C18" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="D18" s="23"/>
+      <c r="E18" s="23"/>
+      <c r="F18" s="23"/>
+      <c r="G18" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="H18" s="12"/>
+      <c r="I18" s="12"/>
+      <c r="J18" s="12"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="B19" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="C19" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="D19" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="E19" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="F19" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="G19" s="17"/>
+      <c r="H19" s="12"/>
+      <c r="I19" s="12"/>
+      <c r="J19" s="12"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="17"/>
+      <c r="B20" s="17"/>
+      <c r="C20" s="17"/>
+      <c r="D20" s="17"/>
+      <c r="E20" s="17"/>
+      <c r="F20" s="17"/>
+      <c r="G20" s="17"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="17"/>
+      <c r="B21" s="17"/>
+      <c r="C21" s="17"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="17"/>
+      <c r="F21" s="17"/>
+      <c r="G21" s="17"/>
+    </row>
+    <row r="22" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A22" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D22" s="4" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A14" s="14"/>
-      <c r="B14" s="16" t="s">
+      <c r="E22" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F22" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="G22" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="A23" s="19"/>
+      <c r="B23" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="C23" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="D23" s="20"/>
+      <c r="E23" s="20"/>
+      <c r="F23" s="20"/>
+      <c r="G23" s="28" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="A24" s="19"/>
+      <c r="B24" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D24" s="4"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="4"/>
+      <c r="G24" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="A25" s="19"/>
+      <c r="B25" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="C25" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="D25" s="20"/>
+      <c r="E25" s="20"/>
+      <c r="F25" s="20"/>
+      <c r="G25" s="28" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A26" s="19"/>
+      <c r="B26" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C14" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="D14" s="16"/>
-      <c r="E14" s="16"/>
-      <c r="F14" s="16"/>
-      <c r="G14" s="16"/>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A15" s="14"/>
-      <c r="B15" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C15" s="2" t="s">
+      <c r="C26" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A16" s="14"/>
-      <c r="B16" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="C16" s="16" t="s">
+      <c r="D26" s="4"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="4"/>
+      <c r="G26" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="A27" s="19"/>
+      <c r="B27" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="C27" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="D16" s="16"/>
-      <c r="E16" s="16"/>
-      <c r="F16" s="16"/>
-      <c r="G16" s="16"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="14"/>
-      <c r="B17" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="C17" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="D17" s="17"/>
-      <c r="E17" s="17"/>
-      <c r="F17" s="17"/>
-      <c r="G17" s="17"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="14"/>
-      <c r="B18" s="16" t="s">
+      <c r="D27" s="20"/>
+      <c r="E27" s="20"/>
+      <c r="F27" s="20"/>
+      <c r="G27" s="28" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A28" s="19"/>
+      <c r="B28" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D28" s="4"/>
+      <c r="E28" s="4"/>
+      <c r="F28" s="4"/>
+      <c r="G28" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A29" s="19"/>
+      <c r="B29" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="C18" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="D18" s="16"/>
-      <c r="E18" s="16"/>
-      <c r="F18" s="16"/>
-      <c r="G18" s="16"/>
-      <c r="H18" s="11"/>
-      <c r="I18" s="11"/>
-      <c r="J18" s="11"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="15"/>
-      <c r="B19" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="C19" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="D19" s="19"/>
-      <c r="E19" s="19"/>
-      <c r="F19" s="19"/>
-      <c r="G19" s="19"/>
-      <c r="H19" s="11"/>
-      <c r="I19" s="11"/>
-      <c r="J19" s="11"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="B20" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="C20" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="D20" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="E20" s="18"/>
-      <c r="F20" s="18"/>
-      <c r="G20" s="18"/>
-      <c r="H20" s="11"/>
-      <c r="I20" s="11"/>
-      <c r="J20" s="11"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="18"/>
-      <c r="B21" s="18"/>
-      <c r="C21" s="18"/>
-      <c r="D21" s="18"/>
-      <c r="E21" s="18"/>
-      <c r="F21" s="18"/>
-      <c r="G21" s="18"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="18"/>
-      <c r="B22" s="18"/>
-      <c r="C22" s="18"/>
-      <c r="D22" s="18"/>
-      <c r="E22" s="18"/>
-      <c r="F22" s="18"/>
-      <c r="G22" s="18"/>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C23" s="3" t="s">
+      <c r="C29" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="D23" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="E23" s="3"/>
-      <c r="F23" s="3"/>
-      <c r="G23" s="3"/>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="20"/>
-      <c r="B24" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="C24" s="21" t="s">
+      <c r="D29" s="20"/>
+      <c r="E29" s="20"/>
+      <c r="F29" s="20"/>
+      <c r="G29" s="28" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="A30" s="19"/>
+      <c r="B30" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="C30" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D24" s="21"/>
-      <c r="E24" s="21"/>
-      <c r="F24" s="21"/>
-      <c r="G24" s="21"/>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="20"/>
-      <c r="B25" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
-      <c r="F25" s="3"/>
-      <c r="G25" s="3"/>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="20"/>
-      <c r="B26" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="C26" s="21" t="s">
-        <v>12</v>
-      </c>
-      <c r="D26" s="21"/>
-      <c r="E26" s="21"/>
-      <c r="F26" s="21"/>
-      <c r="G26" s="21"/>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="20"/>
-      <c r="B27" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D27" s="3"/>
-      <c r="E27" s="3"/>
-      <c r="F27" s="3"/>
-      <c r="G27" s="3"/>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" s="20"/>
-      <c r="B28" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="C28" s="21" t="s">
-        <v>12</v>
-      </c>
-      <c r="D28" s="21"/>
-      <c r="E28" s="21"/>
-      <c r="F28" s="21"/>
-      <c r="G28" s="21"/>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" s="20"/>
-      <c r="B29" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D29" s="3"/>
-      <c r="E29" s="3"/>
-      <c r="F29" s="3"/>
-      <c r="G29" s="3"/>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" s="20"/>
-      <c r="B30" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="C30" s="21" t="s">
-        <v>12</v>
-      </c>
-      <c r="D30" s="21"/>
-      <c r="E30" s="21"/>
-      <c r="F30" s="21"/>
-      <c r="G30" s="21"/>
+      <c r="D30" s="22"/>
+      <c r="E30" s="22"/>
+      <c r="F30" s="4"/>
+      <c r="G30" s="5" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" s="20"/>
-      <c r="B31" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D31" s="23"/>
-      <c r="E31" s="23"/>
-      <c r="F31" s="3"/>
-      <c r="G31" s="3"/>
+      <c r="A31" s="13"/>
+      <c r="B31" s="13"/>
+      <c r="C31" s="13"/>
+      <c r="D31" s="13"/>
+      <c r="E31" s="13"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32" s="12"/>
-      <c r="B32" s="12"/>
-      <c r="C32" s="12"/>
-      <c r="D32" s="12"/>
-      <c r="E32" s="12"/>
+      <c r="A32" s="13"/>
+      <c r="B32" s="13"/>
+      <c r="C32" s="13"/>
+      <c r="D32" s="13"/>
+      <c r="E32" s="13"/>
+      <c r="F32" s="13"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="12"/>
-      <c r="B33" s="12"/>
-      <c r="C33" s="12"/>
-      <c r="D33" s="12"/>
-      <c r="E33" s="12"/>
-      <c r="F33" s="12"/>
+      <c r="A33" s="13"/>
+      <c r="B33" s="13"/>
+      <c r="C33" s="13"/>
+      <c r="D33" s="13"/>
+      <c r="E33" s="13"/>
+      <c r="F33" s="13"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="12"/>
-      <c r="B34" s="12"/>
-      <c r="C34" s="12"/>
-      <c r="D34" s="12"/>
-      <c r="E34" s="12"/>
-      <c r="F34" s="12"/>
+      <c r="A34" s="13"/>
+      <c r="B34" s="13"/>
+      <c r="C34" s="13"/>
+      <c r="D34" s="13"/>
+      <c r="E34" s="13"/>
+      <c r="F34" s="13"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="12"/>
-      <c r="B35" s="12"/>
-      <c r="C35" s="12"/>
-      <c r="D35" s="12"/>
-      <c r="E35" s="12"/>
-      <c r="F35" s="12"/>
+      <c r="A35" s="13"/>
+      <c r="B35" s="13"/>
+      <c r="C35" s="13"/>
+      <c r="D35" s="13"/>
+      <c r="E35" s="13"/>
+      <c r="F35" s="13"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="12"/>
-      <c r="B36" s="12"/>
-      <c r="C36" s="12"/>
-      <c r="D36" s="12"/>
-      <c r="E36" s="12"/>
-      <c r="F36" s="12"/>
+      <c r="A36" s="13"/>
+      <c r="B36" s="13"/>
+      <c r="C36" s="13"/>
+      <c r="D36" s="13"/>
+      <c r="E36" s="13"/>
+      <c r="F36" s="13"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="12"/>
-      <c r="B37" s="12"/>
-      <c r="C37" s="12"/>
-      <c r="D37" s="12"/>
-      <c r="E37" s="12"/>
-      <c r="F37" s="12"/>
+      <c r="A37" s="13"/>
+      <c r="B37" s="13"/>
+      <c r="C37" s="13"/>
+      <c r="D37" s="13"/>
+      <c r="E37" s="13"/>
+      <c r="F37" s="13"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="12"/>
-      <c r="B38" s="12"/>
-      <c r="C38" s="12"/>
-      <c r="D38" s="12"/>
-      <c r="E38" s="12"/>
-      <c r="F38" s="12"/>
+      <c r="A38" s="13"/>
+      <c r="B38" s="13"/>
+      <c r="C38" s="13"/>
+      <c r="D38" s="13"/>
+      <c r="E38" s="13"/>
+      <c r="F38" s="13"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="12"/>
-      <c r="B39" s="12"/>
-      <c r="C39" s="12"/>
-      <c r="D39" s="12"/>
-      <c r="E39" s="12"/>
-      <c r="F39" s="12"/>
+      <c r="A39" s="13"/>
+      <c r="B39" s="13"/>
+      <c r="C39" s="13"/>
+      <c r="D39" s="13"/>
+      <c r="E39" s="13"/>
+      <c r="F39" s="13"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="12"/>
-      <c r="B40" s="12"/>
-      <c r="C40" s="12"/>
-      <c r="D40" s="12"/>
-      <c r="E40" s="12"/>
-      <c r="F40" s="12"/>
+      <c r="A40" s="13"/>
+      <c r="B40" s="13"/>
+      <c r="C40" s="13"/>
+      <c r="D40" s="13"/>
+      <c r="E40" s="13"/>
+      <c r="F40" s="13"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="12"/>
-      <c r="B41" s="12"/>
-      <c r="C41" s="12"/>
-      <c r="D41" s="12"/>
-      <c r="E41" s="12"/>
-      <c r="F41" s="12"/>
+      <c r="A41" s="13"/>
+      <c r="B41" s="13"/>
+      <c r="C41" s="13"/>
+      <c r="D41" s="13"/>
+      <c r="E41" s="13"/>
+      <c r="F41" s="13"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="12"/>
-      <c r="B42" s="12"/>
-      <c r="C42" s="12"/>
-      <c r="D42" s="12"/>
-      <c r="E42" s="12"/>
-      <c r="F42" s="12"/>
+      <c r="A42" s="13"/>
+      <c r="B42" s="13"/>
+      <c r="C42" s="13"/>
+      <c r="D42" s="13"/>
+      <c r="E42" s="13"/>
+      <c r="F42" s="13"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="12"/>
-      <c r="B43" s="12"/>
-      <c r="C43" s="12"/>
-      <c r="D43" s="12"/>
-      <c r="E43" s="12"/>
-      <c r="F43" s="12"/>
+      <c r="A43" s="13"/>
+      <c r="B43" s="13"/>
+      <c r="C43" s="13"/>
+      <c r="D43" s="13"/>
+      <c r="E43" s="13"/>
+      <c r="F43" s="13"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="12"/>
-      <c r="B44" s="12"/>
-      <c r="C44" s="12"/>
-      <c r="D44" s="12"/>
-      <c r="E44" s="12"/>
-      <c r="F44" s="12"/>
+      <c r="A44" s="13"/>
+      <c r="B44" s="13"/>
+      <c r="C44" s="13"/>
+      <c r="D44" s="13"/>
+      <c r="E44" s="13"/>
+      <c r="F44" s="13"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="12"/>
-      <c r="B45" s="12"/>
-      <c r="C45" s="12"/>
-      <c r="D45" s="12"/>
-      <c r="E45" s="12"/>
-      <c r="F45" s="12"/>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="12"/>
-      <c r="B46" s="12"/>
-      <c r="C46" s="12"/>
-      <c r="D46" s="12"/>
-      <c r="E46" s="12"/>
-      <c r="F46" s="12"/>
+      <c r="A45" s="13"/>
+      <c r="B45" s="13"/>
+      <c r="C45" s="13"/>
+      <c r="D45" s="13"/>
+      <c r="E45" s="13"/>
+      <c r="F45" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="D20:D22"/>
-    <mergeCell ref="E20:E22"/>
-    <mergeCell ref="F20:F22"/>
-    <mergeCell ref="G20:G22"/>
-    <mergeCell ref="A23:A31"/>
+    <mergeCell ref="D19:D21"/>
+    <mergeCell ref="E19:E21"/>
+    <mergeCell ref="F19:F21"/>
+    <mergeCell ref="G19:G21"/>
+    <mergeCell ref="A22:A30"/>
     <mergeCell ref="A2:A7"/>
     <mergeCell ref="A8:A11"/>
-    <mergeCell ref="A12:A19"/>
-    <mergeCell ref="A20:A22"/>
-    <mergeCell ref="B20:B22"/>
-    <mergeCell ref="C20:C22"/>
+    <mergeCell ref="A12:A18"/>
+    <mergeCell ref="A19:A21"/>
+    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="C19:C21"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{24FD22E6-9CDE-4D49-B194-D2C49C14D557}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Docs: se corrigio el codigo  de SQL respecto al codigo al darle permisos
</commit_message>
<xml_diff>
--- a/Creacion de users.xlsx
+++ b/Creacion de users.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lucho\Documents\GitHub\Repositorio-de-equipo-3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{002A0ED4-EC8D-4178-B795-9F22E27D4D41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8480CFDD-41F5-46A5-A928-20CC08EB9414}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14775" yWindow="0" windowWidth="14130" windowHeight="16305" xr2:uid="{915D0D72-919F-4EC8-B87C-0E661B558825}"/>
+    <workbookView xWindow="14775" yWindow="0" windowWidth="14130" windowHeight="16290" xr2:uid="{915D0D72-919F-4EC8-B87C-0E661B558825}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -132,93 +132,33 @@
     <t>rositarpelea100</t>
   </si>
   <si>
-    <t>GRANT SELECT, UPDATE ON sena.aprendiz TO 'rositarpelea100'@'localhost'; FLUSH PRIVILEGES;</t>
-  </si>
-  <si>
     <t>GRANT SELECT, UPDATE ON sena.asistencia TO 'rositarpelea100'@'localhost'; FLUSH PRIVILEGES;</t>
   </si>
   <si>
     <t>GRANT SELECT, UPDATE ON sena.incidente TO 'rositarpelea100'@'localhost'; FLUSH PRIVILEGES;</t>
   </si>
   <si>
-    <t>GRANT SELECT, UPDATE ON sena.programas TO 'rositarpelea100'@'localhost'; FLUSH PRIVILEGES;</t>
-  </si>
-  <si>
-    <t>GRANT SELECT, UPDATE ON sena.jornada TO 'rositarpelea100'@'localhost'; FLUSH PRIVILEGES;</t>
-  </si>
-  <si>
-    <t>GRANT SELECT, UPDATE ON sena.modalidad TO 'rositarpelea100'@'localhost'; FLUSH PRIVILEGES;</t>
-  </si>
-  <si>
     <t>santiago.cruzuwu25</t>
   </si>
   <si>
-    <t>GRANT SELECT, UPDATE ON sena.registro_minuta TO 'santiago.cruzuwu25'@'localhost'; FLUSH PRIVILEGES;</t>
-  </si>
-  <si>
     <t>GRANT SELECT, UPDATE ON sena.incidente TO 'santiago.cruzuwu25'@'localhost'; FLUSH PRIVILEGES;</t>
   </si>
   <si>
     <t>GRANT SELECT, UPDATE ON sena.ambiente TO 'santiago.cruzuwu25'@'localhost'; FLUSH PRIVILEGES;</t>
   </si>
   <si>
-    <t>GRANT SELECT, UPDATE ON sena.recursos TO 'santiago.cruzuwu25'@'localhost'; FLUSH PRIVILEGES;</t>
-  </si>
-  <si>
     <t>jtavarez92</t>
   </si>
   <si>
-    <t>GRANT SELECT, UPDATE ON sena.aprendiz TO 'jtavarez92'@'localhost'; FLUSH PRIVILEGES;</t>
-  </si>
-  <si>
     <t>GRANT SELECT, UPDATE ON sena.ambiente TO 'jtavarez92'@'localhost'; FLUSH PRIVILEGES;</t>
   </si>
   <si>
-    <t>GRANT SELECT, UPDATE ON sena.minutas TO 'jtavarez92'@'localhost'; FLUSH PRIVILEGES;</t>
-  </si>
-  <si>
-    <t>GRANT SELECT, UPDATE ON sena.incidente TO 'jtavarez92'@'localhost'; FLUSH PRIVILEGES;</t>
-  </si>
-  <si>
     <t>GRANT SELECT, UPDATE ON sena.asistencia TO 'jtavarez92'@'localhost'; FLUSH PRIVILEGES;</t>
   </si>
   <si>
-    <t>GRANT SELECT, UPDATE ON sena.jornada TO 'jtavarez92'@'localhost'; FLUSH PRIVILEGES;</t>
-  </si>
-  <si>
-    <t>GRANT SELECT, UPDATE ON sena.recursos TO 'jtavarez92'@'localhost'; FLUSH PRIVILEGES;</t>
-  </si>
-  <si>
     <t>javier.pineda21</t>
   </si>
   <si>
-    <t>GRANT SELECT, UPDATE ON sena.aprendiz TO 'javier.pineda21'@'localhost'; FLUSH PRIVILEGES;</t>
-  </si>
-  <si>
-    <t>GRANT SELECT, UPDATE ON sena.asistencia TO 'javier.pineda21'@'localhost'; FLUSH PRIVILEGES;</t>
-  </si>
-  <si>
-    <t>GRANT SELECT, UPDATE ON sena.programas TO 'javier.pineda21'@'localhost'; FLUSH PRIVILEGES;</t>
-  </si>
-  <si>
-    <t>GRANT SELECT, UPDATE ON sena.incidente TO 'javier.pineda21'@'localhost'; FLUSH PRIVILEGES;</t>
-  </si>
-  <si>
-    <t>GRANT SELECT, UPDATE ON sena.minutas TO 'javier.pineda21'@'localhost'; FLUSH PRIVILEGES;</t>
-  </si>
-  <si>
-    <t>GRANT SELECT, UPDATE ON sena.ambiente TO 'javier.pineda21'@'localhost'; FLUSH PRIVILEGES;</t>
-  </si>
-  <si>
-    <t>GRANT SELECT, UPDATE ON sena.recursos TO 'javier.pineda21'@'localhost'; FLUSH PRIVILEGES;</t>
-  </si>
-  <si>
-    <t>GRANT SELECT, UPDATE ON sena.jornada TO 'javier.pineda21'@'localhost'; FLUSH PRIVILEGES;</t>
-  </si>
-  <si>
-    <t>GRANT SELECT, UPDATE ON sena.modalidad TO 'javier.pineda21'@'localhost'; FLUSH PRIVILEGES;</t>
-  </si>
-  <si>
     <t>Adm!nR01@8</t>
   </si>
   <si>
@@ -241,6 +181,66 @@
   </si>
   <si>
     <t>CREATE USER 'javier.pineda21'@'localhost' IDENTIFIED BY 'Instruc@321!';</t>
+  </si>
+  <si>
+    <t>GRANT SELECT ON sena.aprendiz TO 'rositarpelea100'@'localhost'; FLUSH PRIVILEGES;</t>
+  </si>
+  <si>
+    <t>GRANT SELECT ON sena.programas TO 'rositarpelea100'@'localhost'; FLUSH PRIVILEGES;</t>
+  </si>
+  <si>
+    <t>GRANT SELECT ON sena.jornada TO 'rositarpelea100'@'localhost'; FLUSH PRIVILEGES;</t>
+  </si>
+  <si>
+    <t>GRANT SELECT ON sena.modalidad TO 'rositarpelea100'@'localhost'; FLUSH PRIVILEGES;</t>
+  </si>
+  <si>
+    <t>GRANT CREATE, SELECT, UPDATE ON sena.registro_minuta TO 'santiago.cruzuwu25'@'localhost'; FLUSH PRIVILEGES;</t>
+  </si>
+  <si>
+    <t>GRANT SELECT ON sena.recursos TO 'santiago.cruzuwu25'@'localhost'; FLUSH PRIVILEGES;</t>
+  </si>
+  <si>
+    <t>GRANT SELECT ON sena.aprendiz TO 'jtavarez92'@'localhost'; FLUSH PRIVILEGES;</t>
+  </si>
+  <si>
+    <t>GRANT SELECT ON sena.minutas TO 'jtavarez92'@'localhost'; FLUSH PRIVILEGES;</t>
+  </si>
+  <si>
+    <t>GRANT CREATE SELECT, UPDATE ON sena.incidente TO 'jtavarez92'@'localhost'; FLUSH PRIVILEGES;</t>
+  </si>
+  <si>
+    <t>GRANT SELECT ON sena.jornada TO 'jtavarez92'@'localhost'; FLUSH PRIVILEGES;</t>
+  </si>
+  <si>
+    <t>GRANT SELECT ON sena.recursos TO 'jtavarez92'@'localhost'; FLUSH PRIVILEGES;</t>
+  </si>
+  <si>
+    <t>GRANT CREATE,SELECT, UPDATE ON sena.aprendiz TO 'javier.pineda21'@'localhost'; FLUSH PRIVILEGES;</t>
+  </si>
+  <si>
+    <t>GRANT CREATE, SELECT, UPDATE ON sena.asistencia TO 'javier.pineda21'@'localhost'; FLUSH PRIVILEGES;</t>
+  </si>
+  <si>
+    <t>GRANT CREATE, SELECT, UPDATE ON sena.programas TO 'javier.pineda21'@'localhost'; FLUSH PRIVILEGES;</t>
+  </si>
+  <si>
+    <t>GRANT CREATE, SELECT, UPDATE ON sena.incidente TO 'javier.pineda21'@'localhost'; FLUSH PRIVILEGES;</t>
+  </si>
+  <si>
+    <t>GRANT CREATE, SELECT, UPDATE ON sena.minutas TO 'javier.pineda21'@'localhost'; FLUSH PRIVILEGES;</t>
+  </si>
+  <si>
+    <t>GRANT CREATE, SELECT, UPDATE ON sena.ambiente TO 'javier.pineda21'@'localhost'; FLUSH PRIVILEGES;</t>
+  </si>
+  <si>
+    <t>GRANT CREATE, SELECT, UPDATE ON sena.recursos TO 'javier.pineda21'@'localhost'; FLUSH PRIVILEGES;</t>
+  </si>
+  <si>
+    <t>GRANTCREATE, SELECT, UPDATE ON sena.jornada TO 'javier.pineda21'@'localhost'; FLUSH PRIVILEGES;</t>
+  </si>
+  <si>
+    <t>GRANT CREATE, SELECT, UPDATE ON sena.modalidad TO 'javier.pineda21'@'localhost'; FLUSH PRIVILEGES;</t>
   </si>
 </sst>
 </file>
@@ -805,8 +805,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{914852BE-CF9F-4359-89B7-1C4A7749B8FD}">
   <dimension ref="A1:P30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" topLeftCell="B16" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -862,13 +862,13 @@
         <v>31</v>
       </c>
       <c r="E2" s="17" t="s">
-        <v>61</v>
+        <v>41</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>62</v>
+        <v>42</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>32</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:16" ht="60" x14ac:dyDescent="0.25">
@@ -883,7 +883,7 @@
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
       <c r="G3" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:16" ht="60" x14ac:dyDescent="0.25">
@@ -898,10 +898,10 @@
       <c r="E4" s="8"/>
       <c r="F4" s="8"/>
       <c r="G4" s="7" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" ht="60" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="21"/>
       <c r="B5" s="4" t="s">
         <v>17</v>
@@ -913,7 +913,7 @@
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
       <c r="G5" s="3" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:16" ht="45" x14ac:dyDescent="0.25">
@@ -928,10 +928,10 @@
       <c r="E6" s="8"/>
       <c r="F6" s="8"/>
       <c r="G6" s="7" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" ht="60" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="21"/>
       <c r="B7" s="4" t="s">
         <v>19</v>
@@ -943,7 +943,7 @@
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
       <c r="G7" s="3" t="s">
-        <v>37</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:16" ht="60" x14ac:dyDescent="0.25">
@@ -957,16 +957,16 @@
         <v>9</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>63</v>
+        <v>43</v>
       </c>
       <c r="F8" s="15" t="s">
-        <v>64</v>
+        <v>44</v>
       </c>
       <c r="G8" s="15" t="s">
-        <v>39</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:16" ht="60" x14ac:dyDescent="0.25">
@@ -981,7 +981,7 @@
       <c r="E9" s="4"/>
       <c r="F9" s="3"/>
       <c r="G9" s="3" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:16" ht="60" x14ac:dyDescent="0.25">
@@ -996,7 +996,7 @@
       <c r="E10" s="9"/>
       <c r="F10" s="9"/>
       <c r="G10" s="15" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:16" ht="45" x14ac:dyDescent="0.25">
@@ -1011,7 +1011,7 @@
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
       <c r="G11" s="3" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
     </row>
     <row r="12" spans="1:16" ht="45" x14ac:dyDescent="0.25">
@@ -1025,16 +1025,16 @@
         <v>20</v>
       </c>
       <c r="D12" s="14" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="E12" s="14" t="s">
-        <v>65</v>
+        <v>45</v>
       </c>
       <c r="F12" s="14" t="s">
-        <v>66</v>
+        <v>46</v>
       </c>
       <c r="G12" s="14" t="s">
-        <v>44</v>
+        <v>55</v>
       </c>
     </row>
     <row r="13" spans="1:16" ht="60" x14ac:dyDescent="0.25">
@@ -1049,7 +1049,7 @@
       <c r="E13" s="3"/>
       <c r="F13" s="4"/>
       <c r="G13" s="3" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="P13" t="s">
         <v>28</v>
@@ -1067,7 +1067,7 @@
       <c r="E14" s="14"/>
       <c r="F14" s="14"/>
       <c r="G14" s="14" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
     </row>
     <row r="15" spans="1:16" ht="60" x14ac:dyDescent="0.25">
@@ -1082,7 +1082,7 @@
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
       <c r="G15" s="3" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
     </row>
     <row r="16" spans="1:16" ht="60" x14ac:dyDescent="0.25">
@@ -1097,7 +1097,7 @@
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="14" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -1112,7 +1112,7 @@
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
       <c r="G17" s="3" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -1127,7 +1127,7 @@
       <c r="E18" s="14"/>
       <c r="F18" s="14"/>
       <c r="G18" s="14" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -1169,7 +1169,7 @@
       <c r="F21" s="19"/>
       <c r="G21" s="19"/>
     </row>
-    <row r="22" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A22" s="20" t="s">
         <v>8</v>
       </c>
@@ -1180,16 +1180,16 @@
         <v>9</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>67</v>
+        <v>47</v>
       </c>
       <c r="F22" s="16" t="s">
-        <v>68</v>
+        <v>48</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="60" x14ac:dyDescent="0.25">
@@ -1204,7 +1204,7 @@
       <c r="E23" s="11"/>
       <c r="F23" s="11"/>
       <c r="G23" s="18" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="60" x14ac:dyDescent="0.25">
@@ -1219,7 +1219,7 @@
       <c r="E24" s="4"/>
       <c r="F24" s="4"/>
       <c r="G24" s="3" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="60" x14ac:dyDescent="0.25">
@@ -1234,10 +1234,10 @@
       <c r="E25" s="11"/>
       <c r="F25" s="11"/>
       <c r="G25" s="18" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A26" s="20"/>
       <c r="B26" s="4" t="s">
         <v>26</v>
@@ -1249,7 +1249,7 @@
       <c r="E26" s="4"/>
       <c r="F26" s="4"/>
       <c r="G26" s="3" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="60" x14ac:dyDescent="0.25">
@@ -1264,10 +1264,10 @@
       <c r="E27" s="11"/>
       <c r="F27" s="11"/>
       <c r="G27" s="18" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A28" s="20"/>
       <c r="B28" s="4" t="s">
         <v>25</v>
@@ -1279,10 +1279,10 @@
       <c r="E28" s="4"/>
       <c r="F28" s="4"/>
       <c r="G28" s="3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A29" s="20"/>
       <c r="B29" s="11" t="s">
         <v>18</v>
@@ -1294,7 +1294,7 @@
       <c r="E29" s="11"/>
       <c r="F29" s="11"/>
       <c r="G29" s="18" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="60" x14ac:dyDescent="0.25">
@@ -1309,7 +1309,7 @@
       <c r="E30" s="13"/>
       <c r="F30" s="4"/>
       <c r="G30" s="3" t="s">
-        <v>60</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Docs: Se adjuntan las capturas requeridas
</commit_message>
<xml_diff>
--- a/Creacion de users.xlsx
+++ b/Creacion de users.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lucho\Documents\GitHub\Repositorio-de-equipo-3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8480CFDD-41F5-46A5-A928-20CC08EB9414}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D120369E-1E58-4D6B-AA4D-2E2A0F760F72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14775" yWindow="0" windowWidth="14130" windowHeight="16290" xr2:uid="{915D0D72-919F-4EC8-B87C-0E661B558825}"/>
+    <workbookView xWindow="990" yWindow="90" windowWidth="27720" windowHeight="15015" xr2:uid="{915D0D72-919F-4EC8-B87C-0E661B558825}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="71">
   <si>
     <t>TABLAS</t>
   </si>
@@ -241,6 +241,12 @@
   </si>
   <si>
     <t>GRANT CREATE, SELECT, UPDATE ON sena.modalidad TO 'javier.pineda21'@'localhost'; FLUSH PRIVILEGES;</t>
+  </si>
+  <si>
+    <t>PANTALLAZOCODIGO SQL  CREACION USUARIOS</t>
+  </si>
+  <si>
+    <t>VISUALIZACION DE PRIVILEGIOS POR USERS</t>
   </si>
 </sst>
 </file>
@@ -504,6 +510,261 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>489857</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>41416</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>19732</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>503464</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagen 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4233899E-38D0-B07D-D15E-BC52604E9A64}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14341928" y="817023"/>
+          <a:ext cx="7966304" cy="5034048"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>598715</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>27214</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>547007</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>445131</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Imagen 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F6008662-FC09-24BD-9441-2F96F165FA73}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14450786" y="6898821"/>
+          <a:ext cx="7772400" cy="4989917"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>205468</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Imagen 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{12DFDC70-7C9A-B672-8FCF-E44FD5F90428}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="23513143" y="6871607"/>
+          <a:ext cx="7553325" cy="5248275"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>612320</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>40821</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>618</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>285750</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Imagen 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8F85977C-7AD3-27EA-B9D1-7D5CC6D4EBEE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14464391" y="12627428"/>
+          <a:ext cx="7824727" cy="5578929"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>13607</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>44817</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>285750</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Imagen 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{93A9A718-4423-2CB3-8E7F-9AA646C7D095}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="23526750" y="12586607"/>
+          <a:ext cx="7991388" cy="5619750"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -803,10 +1064,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{914852BE-CF9F-4359-89B7-1C4A7749B8FD}">
-  <dimension ref="A1:P30"/>
+  <dimension ref="A1:S30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B16" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="10" workbookViewId="0">
+      <selection activeCell="AI27" sqref="AI27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -819,10 +1080,11 @@
     <col min="6" max="6" width="36.42578125" customWidth="1"/>
     <col min="7" max="7" width="39" customWidth="1"/>
     <col min="8" max="8" width="8.28515625" customWidth="1"/>
-    <col min="10" max="10" width="13.5703125" customWidth="1"/>
+    <col min="10" max="10" width="30.28515625" customWidth="1"/>
+    <col min="12" max="12" width="32" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>2</v>
       </c>
@@ -846,9 +1108,11 @@
       </c>
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-    </row>
-    <row r="2" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+      <c r="L1" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="21" t="s">
         <v>14</v>
       </c>
@@ -871,7 +1135,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="60" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="21"/>
       <c r="B3" s="4" t="s">
         <v>15</v>
@@ -886,7 +1150,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="60" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="21"/>
       <c r="B4" s="8" t="s">
         <v>16</v>
@@ -901,7 +1165,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="21"/>
       <c r="B5" s="4" t="s">
         <v>17</v>
@@ -916,7 +1180,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="21"/>
       <c r="B6" s="8" t="s">
         <v>18</v>
@@ -931,7 +1195,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="21"/>
       <c r="B7" s="4" t="s">
         <v>19</v>
@@ -946,7 +1210,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="8" spans="1:16" ht="60" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" s="22" t="s">
         <v>22</v>
       </c>
@@ -969,7 +1233,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="9" spans="1:16" ht="60" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" s="22"/>
       <c r="B9" s="4" t="s">
         <v>16</v>
@@ -984,7 +1248,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:16" ht="60" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" s="22"/>
       <c r="B10" s="9" t="s">
         <v>24</v>
@@ -998,8 +1262,11 @@
       <c r="G10" s="15" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="11" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+      <c r="L10" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="22"/>
       <c r="B11" s="4" t="s">
         <v>25</v>
@@ -1013,8 +1280,14 @@
       <c r="G11" s="3" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="12" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+      <c r="I11" s="1">
+        <v>1</v>
+      </c>
+      <c r="S11" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="23" t="s">
         <v>6</v>
       </c>
@@ -1037,7 +1310,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="13" spans="1:16" ht="60" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" ht="60" x14ac:dyDescent="0.25">
       <c r="A13" s="24"/>
       <c r="B13" s="3" t="s">
         <v>24</v>
@@ -1055,7 +1328,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="24"/>
       <c r="B14" s="14" t="s">
         <v>26</v>
@@ -1070,7 +1343,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="15" spans="1:16" ht="60" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" ht="60" x14ac:dyDescent="0.25">
       <c r="A15" s="24"/>
       <c r="B15" s="3" t="s">
         <v>16</v>
@@ -1085,7 +1358,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="16" spans="1:16" ht="60" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" ht="60" x14ac:dyDescent="0.25">
       <c r="A16" s="24"/>
       <c r="B16" s="10" t="s">
         <v>15</v>
@@ -1100,7 +1373,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="24"/>
       <c r="B17" s="3" t="s">
         <v>18</v>
@@ -1115,7 +1388,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="25"/>
       <c r="B18" s="14" t="s">
         <v>25</v>
@@ -1130,7 +1403,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" s="19" t="s">
         <v>7</v>
       </c>
@@ -1151,7 +1424,7 @@
       </c>
       <c r="G19" s="19"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20" s="19"/>
       <c r="B20" s="19"/>
       <c r="C20" s="19"/>
@@ -1160,7 +1433,7 @@
       <c r="F20" s="19"/>
       <c r="G20" s="19"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" s="19"/>
       <c r="B21" s="19"/>
       <c r="C21" s="19"/>
@@ -1169,7 +1442,7 @@
       <c r="F21" s="19"/>
       <c r="G21" s="19"/>
     </row>
-    <row r="22" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:19" ht="60" x14ac:dyDescent="0.25">
       <c r="A22" s="20" t="s">
         <v>8</v>
       </c>
@@ -1191,8 +1464,14 @@
       <c r="G22" s="3" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="I22" s="1">
+        <v>3</v>
+      </c>
+      <c r="S22" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" ht="60" x14ac:dyDescent="0.25">
       <c r="A23" s="20"/>
       <c r="B23" s="11" t="s">
         <v>15</v>
@@ -1207,7 +1486,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:19" ht="60" x14ac:dyDescent="0.25">
       <c r="A24" s="20"/>
       <c r="B24" s="4" t="s">
         <v>17</v>
@@ -1222,7 +1501,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:19" ht="60" x14ac:dyDescent="0.25">
       <c r="A25" s="20"/>
       <c r="B25" s="11" t="s">
         <v>16</v>
@@ -1237,7 +1516,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:19" ht="60" x14ac:dyDescent="0.25">
       <c r="A26" s="20"/>
       <c r="B26" s="4" t="s">
         <v>26</v>
@@ -1252,7 +1531,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:19" ht="60" x14ac:dyDescent="0.25">
       <c r="A27" s="20"/>
       <c r="B27" s="11" t="s">
         <v>24</v>
@@ -1267,7 +1546,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:19" ht="60" x14ac:dyDescent="0.25">
       <c r="A28" s="20"/>
       <c r="B28" s="4" t="s">
         <v>25</v>
@@ -1282,7 +1561,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:19" ht="60" x14ac:dyDescent="0.25">
       <c r="A29" s="20"/>
       <c r="B29" s="11" t="s">
         <v>18</v>
@@ -1297,7 +1576,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:19" ht="60" x14ac:dyDescent="0.25">
       <c r="A30" s="20"/>
       <c r="B30" s="12" t="s">
         <v>19</v>
@@ -1330,5 +1609,7 @@
     <hyperlink ref="E2" r:id="rId1" display="M@hilyK2025!" xr:uid="{24FD22E6-9CDE-4D49-B194-D2C49C14D557}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId2"/>
+  <drawing r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Docs: Se corrige el Excel de Creacion de users
</commit_message>
<xml_diff>
--- a/Creacion de users.xlsx
+++ b/Creacion de users.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lucho\Documents\GitHub\Repositorio-de-equipo-3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D120369E-1E58-4D6B-AA4D-2E2A0F760F72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80463B1C-AA8E-4F3E-8E1F-1C9EEFDD8731}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="990" yWindow="90" windowWidth="27720" windowHeight="15015" xr2:uid="{915D0D72-919F-4EC8-B87C-0E661B558825}"/>
+    <workbookView xWindow="885" yWindow="0" windowWidth="21615" windowHeight="15105" xr2:uid="{915D0D72-919F-4EC8-B87C-0E661B558825}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="77">
   <si>
     <t>TABLAS</t>
   </si>
@@ -48,9 +48,6 @@
     <t>CONTRASEÑA</t>
   </si>
   <si>
-    <t>LuisJMarino</t>
-  </si>
-  <si>
     <t>Create, Read, Update, Delete</t>
   </si>
   <si>
@@ -102,9 +99,6 @@
     <t xml:space="preserve">Read </t>
   </si>
   <si>
-    <t>Vigilante Minuta</t>
-  </si>
-  <si>
     <t>Registro minuta</t>
   </si>
   <si>
@@ -123,130 +117,154 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>Vol1Bear_LJM</t>
-  </si>
-  <si>
-    <t>CREATE USER 'santiago.cruzuwu25'@'localhost' IDENTIFIED BY 'Vol1Bear_LJM';</t>
-  </si>
-  <si>
-    <t>rositarpelea100</t>
-  </si>
-  <si>
-    <t>GRANT SELECT, UPDATE ON sena.asistencia TO 'rositarpelea100'@'localhost'; FLUSH PRIVILEGES;</t>
-  </si>
-  <si>
-    <t>GRANT SELECT, UPDATE ON sena.incidente TO 'rositarpelea100'@'localhost'; FLUSH PRIVILEGES;</t>
-  </si>
-  <si>
-    <t>santiago.cruzuwu25</t>
-  </si>
-  <si>
-    <t>GRANT SELECT, UPDATE ON sena.incidente TO 'santiago.cruzuwu25'@'localhost'; FLUSH PRIVILEGES;</t>
-  </si>
-  <si>
-    <t>GRANT SELECT, UPDATE ON sena.ambiente TO 'santiago.cruzuwu25'@'localhost'; FLUSH PRIVILEGES;</t>
-  </si>
-  <si>
-    <t>jtavarez92</t>
-  </si>
-  <si>
-    <t>GRANT SELECT, UPDATE ON sena.ambiente TO 'jtavarez92'@'localhost'; FLUSH PRIVILEGES;</t>
-  </si>
-  <si>
-    <t>GRANT SELECT, UPDATE ON sena.asistencia TO 'jtavarez92'@'localhost'; FLUSH PRIVILEGES;</t>
-  </si>
-  <si>
-    <t>javier.pineda21</t>
-  </si>
-  <si>
-    <t>Adm!nR01@8</t>
-  </si>
-  <si>
-    <t>CREATE USER 'rositarpelea100'@'localhost' IDENTIFIED BY 'Adm!nR01@8';</t>
-  </si>
-  <si>
-    <t>Aprz#2025xy!</t>
-  </si>
-  <si>
-    <t>CREATE USER 'santiago.cruzuwu25'@'localhost' IDENTIFIED BY 'Aprz#2025xy!';</t>
-  </si>
-  <si>
-    <t>Vgs3cuR@9!</t>
-  </si>
-  <si>
-    <t>CREATE USER 'jtavarez92'@'localhost' IDENTIFIED BY 'Vgs3cuR@9!';</t>
-  </si>
-  <si>
-    <t>Instruc@321!</t>
-  </si>
-  <si>
-    <t>CREATE USER 'javier.pineda21'@'localhost' IDENTIFIED BY 'Instruc@321!';</t>
-  </si>
-  <si>
-    <t>GRANT SELECT ON sena.aprendiz TO 'rositarpelea100'@'localhost'; FLUSH PRIVILEGES;</t>
-  </si>
-  <si>
-    <t>GRANT SELECT ON sena.programas TO 'rositarpelea100'@'localhost'; FLUSH PRIVILEGES;</t>
-  </si>
-  <si>
-    <t>GRANT SELECT ON sena.jornada TO 'rositarpelea100'@'localhost'; FLUSH PRIVILEGES;</t>
-  </si>
-  <si>
-    <t>GRANT SELECT ON sena.modalidad TO 'rositarpelea100'@'localhost'; FLUSH PRIVILEGES;</t>
-  </si>
-  <si>
-    <t>GRANT CREATE, SELECT, UPDATE ON sena.registro_minuta TO 'santiago.cruzuwu25'@'localhost'; FLUSH PRIVILEGES;</t>
-  </si>
-  <si>
-    <t>GRANT SELECT ON sena.recursos TO 'santiago.cruzuwu25'@'localhost'; FLUSH PRIVILEGES;</t>
-  </si>
-  <si>
-    <t>GRANT SELECT ON sena.aprendiz TO 'jtavarez92'@'localhost'; FLUSH PRIVILEGES;</t>
-  </si>
-  <si>
-    <t>GRANT SELECT ON sena.minutas TO 'jtavarez92'@'localhost'; FLUSH PRIVILEGES;</t>
-  </si>
-  <si>
-    <t>GRANT CREATE SELECT, UPDATE ON sena.incidente TO 'jtavarez92'@'localhost'; FLUSH PRIVILEGES;</t>
-  </si>
-  <si>
-    <t>GRANT SELECT ON sena.jornada TO 'jtavarez92'@'localhost'; FLUSH PRIVILEGES;</t>
-  </si>
-  <si>
-    <t>GRANT SELECT ON sena.recursos TO 'jtavarez92'@'localhost'; FLUSH PRIVILEGES;</t>
-  </si>
-  <si>
-    <t>GRANT CREATE,SELECT, UPDATE ON sena.aprendiz TO 'javier.pineda21'@'localhost'; FLUSH PRIVILEGES;</t>
-  </si>
-  <si>
-    <t>GRANT CREATE, SELECT, UPDATE ON sena.asistencia TO 'javier.pineda21'@'localhost'; FLUSH PRIVILEGES;</t>
-  </si>
-  <si>
-    <t>GRANT CREATE, SELECT, UPDATE ON sena.programas TO 'javier.pineda21'@'localhost'; FLUSH PRIVILEGES;</t>
-  </si>
-  <si>
-    <t>GRANT CREATE, SELECT, UPDATE ON sena.incidente TO 'javier.pineda21'@'localhost'; FLUSH PRIVILEGES;</t>
-  </si>
-  <si>
-    <t>GRANT CREATE, SELECT, UPDATE ON sena.minutas TO 'javier.pineda21'@'localhost'; FLUSH PRIVILEGES;</t>
-  </si>
-  <si>
-    <t>GRANT CREATE, SELECT, UPDATE ON sena.ambiente TO 'javier.pineda21'@'localhost'; FLUSH PRIVILEGES;</t>
-  </si>
-  <si>
-    <t>GRANT CREATE, SELECT, UPDATE ON sena.recursos TO 'javier.pineda21'@'localhost'; FLUSH PRIVILEGES;</t>
-  </si>
-  <si>
-    <t>GRANTCREATE, SELECT, UPDATE ON sena.jornada TO 'javier.pineda21'@'localhost'; FLUSH PRIVILEGES;</t>
-  </si>
-  <si>
-    <t>GRANT CREATE, SELECT, UPDATE ON sena.modalidad TO 'javier.pineda21'@'localhost'; FLUSH PRIVILEGES;</t>
-  </si>
-  <si>
     <t>PANTALLAZOCODIGO SQL  CREACION USUARIOS</t>
   </si>
   <si>
     <t>VISUALIZACION DE PRIVILEGIOS POR USERS</t>
+  </si>
+  <si>
+    <t>luis.vargas</t>
+  </si>
+  <si>
+    <t>GRANT ALL PRIVILEGES ON mydb.* TO 'luis.vargas'@'localhost' WITH GRANT OPTION;</t>
+  </si>
+  <si>
+    <t>KennerStorm#SC</t>
+  </si>
+  <si>
+    <t>carlos.garcia</t>
+  </si>
+  <si>
+    <t>GRANT CREATE,SELECT, UPDATE ON sena.aprendiz TO 'carlos.garcia'@'localhost'; FLUSH PRIVILEGES;</t>
+  </si>
+  <si>
+    <t>GRANT CREATE, SELECT, UPDATE ON sena.asistencia TO 'carlos.garcia'@'localhost'; FLUSH PRIVILEGES;</t>
+  </si>
+  <si>
+    <t>GRANT CREATE, SELECT, UPDATE ON sena.programas TO 'carlos.garcia'@'localhost'; FLUSH PRIVILEGES;</t>
+  </si>
+  <si>
+    <t>GRANT CREATE, SELECT, UPDATE ON sena.incidente TO 'carlos.garcia'@'localhost'; FLUSH PRIVILEGES;</t>
+  </si>
+  <si>
+    <t>GRANT CREATE, SELECT, UPDATE ON sena.minutas TO 'carlos.garcia'@'localhost'; FLUSH PRIVILEGES;</t>
+  </si>
+  <si>
+    <t>GRANT CREATE, SELECT, UPDATE ON sena.ambiente TO 'carlos.garcia'@'localhost'; FLUSH PRIVILEGES;</t>
+  </si>
+  <si>
+    <t>GRANT CREATE, SELECT, UPDATE ON sena.recursos TO 'carlos.garcia'@'localhost'; FLUSH PRIVILEGES;</t>
+  </si>
+  <si>
+    <t>GRANTCREATE, SELECT, UPDATE ON sena.jornada TO 'carlos.garcia'@'localhost'; FLUSH PRIVILEGES;</t>
+  </si>
+  <si>
+    <t>GRANT CREATE, SELECT, UPDATE ON sena.modalidad TO 'carlos.garcia'@'localhost'; FLUSH PRIVILEGES;</t>
+  </si>
+  <si>
+    <t>C@rlosC0ord#25</t>
+  </si>
+  <si>
+    <t>CREATE USER 'carlos.garcia'@'localhost' IDENTIFIED BY 'C@rlosC0ord#25';</t>
+  </si>
+  <si>
+    <t>gloria.parra</t>
+  </si>
+  <si>
+    <t>GRANT SELECT ON sena.aprendiz TO 'gloria.parra'@'localhost'; FLUSH PRIVILEGES;</t>
+  </si>
+  <si>
+    <t>GRANT SELECT, UPDATE ON sena.asistencia TO 'gloria.parra'@'localhost'; FLUSH PRIVILEGES;</t>
+  </si>
+  <si>
+    <t>GRANT SELECT, UPDATE ON sena.incidente TO 'gloria.parra'@'localhost'; FLUSH PRIVILEGES;</t>
+  </si>
+  <si>
+    <t>GRANT SELECT ON sena.programas TO 'gloria.parra'@'localhost'; FLUSH PRIVILEGES;</t>
+  </si>
+  <si>
+    <t>GRANT SELECT ON sena.jornada TO 'gloria.parra'@'localhost'; FLUSH PRIVILEGES;</t>
+  </si>
+  <si>
+    <t>GRANT SELECT ON sena.modalidad TO 'gloria.parra'@'localhost'; FLUSH PRIVILEGES;</t>
+  </si>
+  <si>
+    <t>M@hilyK2025!</t>
+  </si>
+  <si>
+    <t>CREATE USER 'gloria.parra'@'localhost' IDENTIFIED BY 'M@hilyK2025!';</t>
+  </si>
+  <si>
+    <t>Guarda de seguridad</t>
+  </si>
+  <si>
+    <t>rosa.arango</t>
+  </si>
+  <si>
+    <t>GRANT CREATE, SELECT, UPDATE ON sena.registro_minuta TO 'rosa.arango'@'localhost'; FLUSH PRIVILEGES;</t>
+  </si>
+  <si>
+    <t>GRANT SELECT, UPDATE ON sena.incidente TO 'rosa.arango'@'localhost'; FLUSH PRIVILEGES;</t>
+  </si>
+  <si>
+    <t>GRANT SELECT, UPDATE ON sena.ambiente TO 'rosa.arango'@'localhost'; FLUSH PRIVILEGES;</t>
+  </si>
+  <si>
+    <t>GRANT SELECT ON sena.recursos TO 'rosa.arango'@'localhost'; FLUSH PRIVILEGES;</t>
+  </si>
+  <si>
+    <t>CREATE USER 'rosa.arango'@'localhost' IDENTIFIED BY 'KennerStorm#SC';</t>
+  </si>
+  <si>
+    <t>D4v1dSC#08</t>
+  </si>
+  <si>
+    <t>CREATE USER 'rosa.arango'@'localhost' IDENTIFIED BY 'D4v1dSC#08';</t>
+  </si>
+  <si>
+    <t>andres.rojas</t>
+  </si>
+  <si>
+    <t>GRANT SELECT ON sena.aprendiz TO 'andres.rojas'@'localhost'; FLUSH PRIVILEGES;</t>
+  </si>
+  <si>
+    <t>GRANT SELECT, UPDATE ON sena.ambiente TO 'andres.rojas'@'localhost'; FLUSH PRIVILEGES;</t>
+  </si>
+  <si>
+    <t>GRANT SELECT ON sena.minutas TO 'andres.rojas'@'localhost'; FLUSH PRIVILEGES;</t>
+  </si>
+  <si>
+    <t>GRANT CREATE SELECT, UPDATE ON sena.incidente TO 'andres.rojas'@'localhost'; FLUSH PRIVILEGES;</t>
+  </si>
+  <si>
+    <t>GRANT SELECT, UPDATE ON sena.asistencia TO 'andres.rojas'@'localhost'; FLUSH PRIVILEGES;</t>
+  </si>
+  <si>
+    <t>GRANT SELECT ON sena.jornada TO 'andres.rojas'@'localhost'; FLUSH PRIVILEGES;</t>
+  </si>
+  <si>
+    <t>GRANT SELECT ON sena.recursos TO 'andres.rojas'@'localhost'; FLUSH PRIVILEGES;</t>
+  </si>
+  <si>
+    <t>E.CamiloA$92</t>
+  </si>
+  <si>
+    <t>CREATE USER 'andres.rojas'@'localhost' IDENTIFIED BY 'E.CamiloA$92';</t>
+  </si>
+  <si>
+    <t>ADMINISTRADOR</t>
+  </si>
+  <si>
+    <t>APRENDIZ</t>
+  </si>
+  <si>
+    <t>COORDINADOR</t>
+  </si>
+  <si>
+    <t>GUARDA DE SEGURIDAD</t>
+  </si>
+  <si>
+    <t>INSTRUCTOR</t>
   </si>
 </sst>
 </file>
@@ -411,7 +429,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -467,25 +485,31 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -516,23 +540,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>489857</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>41416</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>19732</xdr:colOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>34636</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>503464</xdr:rowOff>
+      <xdr:rowOff>391218</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Imagen 2">
+        <xdr:cNvPr id="4" name="Imagen 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4233899E-38D0-B07D-D15E-BC52604E9A64}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1FC3516F-ECC1-3462-8BED-67E4BAEEF513}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -541,21 +565,59 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="14341928" y="817023"/>
-          <a:ext cx="7966304" cy="5034048"/>
+          <a:off x="14443364" y="779318"/>
+          <a:ext cx="7221681" cy="4963218"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>311728</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>398318</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Imagen 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C7AE65D1-4DFC-3BA0-8100-16ECE5107C28}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="22236545" y="779318"/>
+          <a:ext cx="7446819" cy="4970318"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -567,22 +629,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>598715</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>27214</xdr:rowOff>
+      <xdr:colOff>502227</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>51955</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>547007</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>445131</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>428921</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>338011</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Imagen 4">
+        <xdr:cNvPr id="8" name="Imagen 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F6008662-FC09-24BD-9441-2F96F165FA73}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0CFBA8FE-7BD8-728A-033E-181F812F4B8A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -591,21 +653,15 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="14450786" y="6898821"/>
-          <a:ext cx="7772400" cy="4989917"/>
+          <a:off x="14339454" y="7498773"/>
+          <a:ext cx="8326012" cy="2191056"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -618,21 +674,21 @@
     <xdr:from>
       <xdr:col>19</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>31</xdr:col>
-      <xdr:colOff>205468</xdr:colOff>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>398318</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:rowOff>186867</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="7" name="Imagen 6">
+        <xdr:cNvPr id="10" name="Imagen 9">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{12DFDC70-7C9A-B672-8FCF-E44FD5F90428}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D0602CFD-676D-146E-CF75-67966CC3ED99}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -641,21 +697,59 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="23513143" y="6871607"/>
-          <a:ext cx="7553325" cy="5248275"/>
+          <a:off x="23448818" y="7446818"/>
+          <a:ext cx="7533409" cy="4758867"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>44</xdr:col>
+      <xdr:colOff>350976</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>95822</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Imagen 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ADEB2591-BF6F-7CCC-2E99-80BB36D37F00}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="31778864" y="7446818"/>
+          <a:ext cx="8230749" cy="4096322"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -667,22 +761,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>612320</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>40821</xdr:rowOff>
+      <xdr:colOff>415637</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>346364</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>618</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>285750</xdr:rowOff>
+      <xdr:colOff>342331</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>124241</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="9" name="Imagen 8">
+        <xdr:cNvPr id="13" name="Imagen 12">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8F85977C-7AD3-27EA-B9D1-7D5CC6D4EBEE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1FAD4E79-523C-4906-E78B-FA069210C7C2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -691,21 +785,15 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="14464391" y="12627428"/>
-          <a:ext cx="7824727" cy="5578929"/>
+          <a:off x="14252864" y="11222182"/>
+          <a:ext cx="8326012" cy="2981741"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -717,22 +805,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>13607</xdr:colOff>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>21</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>32</xdr:col>
-      <xdr:colOff>44817</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>285750</xdr:rowOff>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>45332</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>191058</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="11" name="Imagen 10">
+        <xdr:cNvPr id="14" name="Imagen 13">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{93A9A718-4423-2CB3-8E7F-9AA646C7D095}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E21455DB-0957-8CB8-5C2A-15FF5DD41235}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -741,21 +829,59 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="23526750" y="12586607"/>
-          <a:ext cx="7991388" cy="5619750"/>
+          <a:off x="23448818" y="13317682"/>
+          <a:ext cx="8392696" cy="4001058"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>225137</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>207818</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>151831</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>75327</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="15" name="Imagen 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AB9845A5-EA93-B5D9-4ACF-DAF21200009C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14062364" y="15811500"/>
+          <a:ext cx="8326012" cy="6154009"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1064,10 +1190,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{914852BE-CF9F-4359-89B7-1C4A7749B8FD}">
-  <dimension ref="A1:S30"/>
+  <dimension ref="A1:T30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="10" workbookViewId="0">
-      <selection activeCell="AI27" sqref="AI27"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="55" zoomScaleNormal="55" zoomScaleSheetLayoutView="10" workbookViewId="0">
+      <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1082,9 +1208,10 @@
     <col min="8" max="8" width="8.28515625" customWidth="1"/>
     <col min="10" max="10" width="30.28515625" customWidth="1"/>
     <col min="12" max="12" width="32" customWidth="1"/>
+    <col min="20" max="20" width="34.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>2</v>
       </c>
@@ -1092,151 +1219,151 @@
         <v>0</v>
       </c>
       <c r="C1" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="6" t="s">
         <v>10</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>11</v>
       </c>
       <c r="E1" s="6" t="s">
         <v>3</v>
       </c>
       <c r="F1" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="6" t="s">
         <v>12</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>13</v>
       </c>
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
       <c r="L1" s="2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="21" t="s">
-        <v>14</v>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="19" t="s">
+        <v>13</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>1</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="E2" s="17" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" ht="60" x14ac:dyDescent="0.25">
-      <c r="A3" s="21"/>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" ht="60" x14ac:dyDescent="0.25">
+      <c r="A3" s="19"/>
       <c r="B3" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
       <c r="G3" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" ht="60" x14ac:dyDescent="0.25">
-      <c r="A4" s="21"/>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" ht="60" x14ac:dyDescent="0.25">
+      <c r="A4" s="19"/>
       <c r="B4" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D4" s="8"/>
       <c r="E4" s="8"/>
       <c r="F4" s="8"/>
       <c r="G4" s="7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="21"/>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="19"/>
       <c r="B5" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
       <c r="G5" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="21"/>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="19"/>
       <c r="B6" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D6" s="8"/>
       <c r="E6" s="8"/>
       <c r="F6" s="8"/>
       <c r="G6" s="7" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="21"/>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="19"/>
       <c r="B7" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>19</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>20</v>
       </c>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
       <c r="G7" s="3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" ht="60" x14ac:dyDescent="0.25">
-      <c r="A8" s="22" t="s">
-        <v>22</v>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" ht="60" x14ac:dyDescent="0.25">
+      <c r="A8" s="20" t="s">
+        <v>53</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>34</v>
+        <v>54</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>43</v>
+        <v>60</v>
       </c>
       <c r="F8" s="15" t="s">
-        <v>44</v>
+        <v>61</v>
       </c>
       <c r="G8" s="15" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" ht="60" x14ac:dyDescent="0.25">
-      <c r="A9" s="22"/>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" ht="60" x14ac:dyDescent="0.25">
+      <c r="A9" s="20"/>
       <c r="B9" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>1</v>
@@ -1245,13 +1372,13 @@
       <c r="E9" s="4"/>
       <c r="F9" s="3"/>
       <c r="G9" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" ht="60" x14ac:dyDescent="0.25">
-      <c r="A10" s="22"/>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" ht="60" x14ac:dyDescent="0.25">
+      <c r="A10" s="20"/>
       <c r="B10" s="9" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C10" s="9" t="s">
         <v>1</v>
@@ -1260,108 +1387,114 @@
       <c r="E10" s="9"/>
       <c r="F10" s="9"/>
       <c r="G10" s="15" t="s">
-        <v>36</v>
+        <v>57</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="11" spans="1:19" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" s="22"/>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="20"/>
       <c r="B11" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
       <c r="G11" s="3" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="I11" s="1">
         <v>1</v>
       </c>
+      <c r="J11" t="s">
+        <v>72</v>
+      </c>
       <c r="S11" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="12" spans="1:19" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12" s="23" t="s">
-        <v>6</v>
+      <c r="T11" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12" s="21" t="s">
+        <v>5</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D12" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="E12" s="14" t="s">
-        <v>45</v>
+        <v>62</v>
+      </c>
+      <c r="E12" s="27" t="s">
+        <v>70</v>
       </c>
       <c r="F12" s="14" t="s">
-        <v>46</v>
+        <v>71</v>
       </c>
       <c r="G12" s="14" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="13" spans="1:19" ht="60" x14ac:dyDescent="0.25">
-      <c r="A13" s="24"/>
+        <v>63</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" ht="60" x14ac:dyDescent="0.25">
+      <c r="A13" s="22"/>
       <c r="B13" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
       <c r="F13" s="4"/>
       <c r="G13" s="3" t="s">
-        <v>38</v>
+        <v>64</v>
       </c>
       <c r="P13" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="14" spans="1:19" ht="45" x14ac:dyDescent="0.25">
-      <c r="A14" s="24"/>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" ht="45" x14ac:dyDescent="0.25">
+      <c r="A14" s="22"/>
       <c r="B14" s="14" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D14" s="14"/>
       <c r="E14" s="14"/>
       <c r="F14" s="14"/>
       <c r="G14" s="14" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="15" spans="1:19" ht="60" x14ac:dyDescent="0.25">
-      <c r="A15" s="24"/>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" ht="60" x14ac:dyDescent="0.25">
+      <c r="A15" s="22"/>
       <c r="B15" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
       <c r="G15" s="3" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="16" spans="1:19" ht="60" x14ac:dyDescent="0.25">
-      <c r="A16" s="24"/>
+        <v>66</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" ht="60" x14ac:dyDescent="0.25">
+      <c r="A16" s="22"/>
       <c r="B16" s="10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C16" s="10" t="s">
         <v>1</v>
@@ -1370,246 +1503,264 @@
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="14" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="17" spans="1:19" ht="45" x14ac:dyDescent="0.25">
-      <c r="A17" s="24"/>
+        <v>67</v>
+      </c>
+      <c r="I16">
+        <v>3</v>
+      </c>
+      <c r="J16" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" ht="45" x14ac:dyDescent="0.25">
+      <c r="A17" s="22"/>
       <c r="B17" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
       <c r="G17" s="3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="18" spans="1:19" ht="45" x14ac:dyDescent="0.25">
-      <c r="A18" s="25"/>
+        <v>68</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" ht="45" x14ac:dyDescent="0.25">
+      <c r="A18" s="23"/>
       <c r="B18" s="14" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D18" s="14"/>
       <c r="E18" s="14"/>
       <c r="F18" s="14"/>
       <c r="G18" s="14" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A19" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="C19" s="24" t="s">
+        <v>4</v>
+      </c>
+      <c r="D19" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="E19" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="F19" s="24" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A19" s="19" t="s">
+      <c r="G19" s="24" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A20" s="24"/>
+      <c r="B20" s="24"/>
+      <c r="C20" s="24"/>
+      <c r="D20" s="24"/>
+      <c r="E20" s="24"/>
+      <c r="F20" s="24"/>
+      <c r="G20" s="24"/>
+    </row>
+    <row r="21" spans="1:20" ht="72" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="24"/>
+      <c r="B21" s="24"/>
+      <c r="C21" s="24"/>
+      <c r="D21" s="24"/>
+      <c r="E21" s="24"/>
+      <c r="F21" s="24"/>
+      <c r="G21" s="24"/>
+      <c r="S21" s="1">
+        <v>4</v>
+      </c>
+      <c r="T21" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" ht="60" x14ac:dyDescent="0.25">
+      <c r="A22" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="B19" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="C19" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="D19" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="E19" s="19" t="s">
-        <v>29</v>
-      </c>
-      <c r="F19" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="G19" s="19"/>
-    </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A20" s="19"/>
-      <c r="B20" s="19"/>
-      <c r="C20" s="19"/>
-      <c r="D20" s="19"/>
-      <c r="E20" s="19"/>
-      <c r="F20" s="19"/>
-      <c r="G20" s="19"/>
-    </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A21" s="19"/>
-      <c r="B21" s="19"/>
-      <c r="C21" s="19"/>
-      <c r="D21" s="19"/>
-      <c r="E21" s="19"/>
-      <c r="F21" s="19"/>
-      <c r="G21" s="19"/>
-    </row>
-    <row r="22" spans="1:19" ht="60" x14ac:dyDescent="0.25">
-      <c r="A22" s="20" t="s">
+      <c r="B22" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C22" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="D22" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E22" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="F22" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="I22" s="1"/>
+    </row>
+    <row r="23" spans="1:20" ht="60" x14ac:dyDescent="0.25">
+      <c r="A23" s="25"/>
+      <c r="B23" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C22" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="F22" s="16" t="s">
-        <v>48</v>
-      </c>
-      <c r="G22" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="I22" s="1">
-        <v>3</v>
-      </c>
-      <c r="S22" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="23" spans="1:19" ht="60" x14ac:dyDescent="0.25">
-      <c r="A23" s="20"/>
-      <c r="B23" s="11" t="s">
-        <v>15</v>
-      </c>
       <c r="C23" s="11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D23" s="11"/>
       <c r="E23" s="11"/>
       <c r="F23" s="11"/>
       <c r="G23" s="18" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="24" spans="1:19" ht="60" x14ac:dyDescent="0.25">
-      <c r="A24" s="20"/>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" ht="60" x14ac:dyDescent="0.25">
+      <c r="A24" s="25"/>
       <c r="B24" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D24" s="4"/>
       <c r="E24" s="4"/>
       <c r="F24" s="4"/>
       <c r="G24" s="3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="25" spans="1:19" ht="60" x14ac:dyDescent="0.25">
-      <c r="A25" s="20"/>
+        <v>35</v>
+      </c>
+      <c r="I24">
+        <v>5</v>
+      </c>
+      <c r="J24" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20" ht="60" x14ac:dyDescent="0.25">
+      <c r="A25" s="25"/>
       <c r="B25" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D25" s="11"/>
       <c r="E25" s="11"/>
       <c r="F25" s="11"/>
       <c r="G25" s="18" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="26" spans="1:19" ht="60" x14ac:dyDescent="0.25">
-      <c r="A26" s="20"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="26" spans="1:20" ht="60" x14ac:dyDescent="0.25">
+      <c r="A26" s="25"/>
       <c r="B26" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D26" s="4"/>
       <c r="E26" s="4"/>
       <c r="F26" s="4"/>
       <c r="G26" s="3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="27" spans="1:19" ht="60" x14ac:dyDescent="0.25">
-      <c r="A27" s="20"/>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20" ht="60" x14ac:dyDescent="0.25">
+      <c r="A27" s="25"/>
       <c r="B27" s="11" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C27" s="11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D27" s="11"/>
       <c r="E27" s="11"/>
       <c r="F27" s="11"/>
       <c r="G27" s="18" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="28" spans="1:19" ht="60" x14ac:dyDescent="0.25">
-      <c r="A28" s="20"/>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="28" spans="1:20" ht="60" x14ac:dyDescent="0.25">
+      <c r="A28" s="25"/>
       <c r="B28" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D28" s="4"/>
       <c r="E28" s="4"/>
       <c r="F28" s="4"/>
       <c r="G28" s="3" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="29" spans="1:19" ht="60" x14ac:dyDescent="0.25">
-      <c r="A29" s="20"/>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="29" spans="1:20" ht="60" x14ac:dyDescent="0.25">
+      <c r="A29" s="25"/>
       <c r="B29" s="11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C29" s="11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D29" s="11"/>
       <c r="E29" s="11"/>
       <c r="F29" s="11"/>
       <c r="G29" s="18" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="30" spans="1:19" ht="60" x14ac:dyDescent="0.25">
-      <c r="A30" s="20"/>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="30" spans="1:20" ht="60" x14ac:dyDescent="0.25">
+      <c r="A30" s="25"/>
       <c r="B30" s="12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D30" s="13"/>
       <c r="E30" s="13"/>
       <c r="F30" s="4"/>
       <c r="G30" s="3" t="s">
-        <v>68</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="I30" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A2:A7"/>
-    <mergeCell ref="A8:A11"/>
-    <mergeCell ref="A12:A18"/>
-    <mergeCell ref="A19:A21"/>
-    <mergeCell ref="B19:B21"/>
     <mergeCell ref="D19:D21"/>
     <mergeCell ref="E19:E21"/>
     <mergeCell ref="F19:F21"/>
     <mergeCell ref="G19:G21"/>
     <mergeCell ref="A22:A30"/>
     <mergeCell ref="C19:C21"/>
+    <mergeCell ref="A2:A7"/>
+    <mergeCell ref="A8:A11"/>
+    <mergeCell ref="A12:A18"/>
+    <mergeCell ref="A19:A21"/>
+    <mergeCell ref="B19:B21"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" display="M@hilyK2025!" xr:uid="{24FD22E6-9CDE-4D49-B194-D2C49C14D557}"/>
+    <hyperlink ref="E2" r:id="rId1" display="Adm!nR01@8" xr:uid="{24FD22E6-9CDE-4D49-B194-D2C49C14D557}"/>
+    <hyperlink ref="E22" r:id="rId2" display="Instruc@321!" xr:uid="{21E68678-509D-4082-AEF8-AEDAC89A49C2}"/>
+    <hyperlink ref="E12" r:id="rId3" display="Vgs3cuR@9!" xr:uid="{859D033F-C813-4362-94B3-B1F81F86AC86}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId2"/>
-  <drawing r:id="rId3"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId4"/>
+  <drawing r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>